<commit_message>
Naprawić wywalanie pętli na "Substation"
</commit_message>
<xml_diff>
--- a/CIM_import_program/powiązania.xlsx
+++ b/CIM_import_program/powiązania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Python_Micro_Codes\CIM_import_program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32333911-9CFE-454C-8341-166E23796994}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBB571A-2EA8-45E5-A864-4A0A95603BF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="53640" yWindow="2280" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="172">
   <si>
     <t>cim:DiscreteValue</t>
   </si>
@@ -462,13 +462,94 @@
   </si>
   <si>
     <t>#67586991</t>
+  </si>
+  <si>
+    <t>_d2f3aceba7fc4314b27144e0010a3f54</t>
+  </si>
+  <si>
+    <t>SN</t>
+  </si>
+  <si>
+    <t>#_aa735c5851f048fa89b4c2f7bab2258a</t>
+  </si>
+  <si>
+    <t>#_5180dd6229c04f688db8f010857a8c13</t>
+  </si>
+  <si>
+    <t>_12e0ccacadd34ccc94f4179746f3be3e</t>
+  </si>
+  <si>
+    <t>NN</t>
+  </si>
+  <si>
+    <t>#_dbd85671a32f41d0be567b9ee5bbd979</t>
+  </si>
+  <si>
+    <t>#BV_6</t>
+  </si>
+  <si>
+    <t>_5180dd6229c04f688db8f010857a8c13</t>
+  </si>
+  <si>
+    <t>T1</t>
+  </si>
+  <si>
+    <t>#_3e67567dfa9443169ecc1ee28ee67f48</t>
+  </si>
+  <si>
+    <t>&lt;-- pojawia się w dużej ilości TransformerEnd</t>
+  </si>
+  <si>
+    <t>Brak połączeń ---</t>
+  </si>
+  <si>
+    <t>_bb2e8a5559524debbec16ed5a45a91b0</t>
+  </si>
+  <si>
+    <t>#_7dcb88942a954fd7befdaa6de1b2216e</t>
+  </si>
+  <si>
+    <t>_75d81f40021841e3b3759224e6eb9558</t>
+  </si>
+  <si>
+    <t>#_bb2e8a5559524debbec16ed5a45a91b0</t>
+  </si>
+  <si>
+    <t>_b8a73c1e5bf443c38cc92c95f1525a54</t>
+  </si>
+  <si>
+    <t>BYŁO</t>
+  </si>
+  <si>
+    <t>_7dcb88942a954fd7befdaa6de1b2216e</t>
+  </si>
+  <si>
+    <t>2OELG_TR1</t>
+  </si>
+  <si>
+    <t>#_2e15e3ee64624e20b40cf70e02292d7a</t>
+  </si>
+  <si>
+    <t>_2e15e3ee64624e20b40cf70e02292d7a</t>
+  </si>
+  <si>
+    <t>2OELG</t>
+  </si>
+  <si>
+    <t>2OELG ELGUM</t>
+  </si>
+  <si>
+    <t>GPZ BÄ\u0098DZIN-2S1989 Chemiczna</t>
+  </si>
+  <si>
+    <t>#_fe72415910bf4d1d8edc4573c2b2ea2a</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -476,8 +557,42 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFDEDEDE"/>
+      <name val="Lucida Console"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -490,8 +605,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -499,13 +626,61 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -786,25 +961,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C6:L36"/>
+  <dimension ref="C6:N90"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="J67" workbookViewId="0">
+      <selection activeCell="M87" sqref="M87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="37.28515625" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="5" max="5" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="35.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.140625" customWidth="1"/>
-    <col min="12" max="12" width="22.85546875" customWidth="1"/>
-    <col min="13" max="13" width="16.5703125" customWidth="1"/>
+    <col min="12" max="12" width="45.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="36.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="3:12" x14ac:dyDescent="0.25">
@@ -866,76 +1041,76 @@
       </c>
     </row>
     <row r="10" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C11">
+      <c r="C11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11">
         <v>67586991</v>
       </c>
-      <c r="D11" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="12" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="C12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
         <v>135</v>
       </c>
-      <c r="D12" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="13" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="C13" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
         <v>136</v>
       </c>
-      <c r="D13" t="s">
-        <v>2</v>
-      </c>
     </row>
     <row r="14" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="C14" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" t="s">
         <v>137</v>
       </c>
-      <c r="D14" t="s">
-        <v>17</v>
-      </c>
     </row>
     <row r="15" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+      <c r="C15" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D15" t="s">
         <v>138</v>
       </c>
-      <c r="D15" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="16" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="C16" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" t="s">
         <v>139</v>
       </c>
-      <c r="D16" t="s">
-        <v>10</v>
-      </c>
     </row>
     <row r="17" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="C17" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" t="s">
         <v>140</v>
       </c>
-      <c r="D17" t="s">
+    </row>
+    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C18" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D18" t="s">
-        <v>19</v>
-      </c>
-    </row>
     <row r="19" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="D19" t="s">
+      <c r="C19" s="6" t="s">
         <v>19</v>
       </c>
     </row>
@@ -957,62 +1132,513 @@
       </c>
     </row>
     <row r="29" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C29" t="s">
+      <c r="C29" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="D29" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="30" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C30" t="s">
+      <c r="C30" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D30" t="s">
         <v>141</v>
       </c>
-      <c r="D30" t="s">
+    </row>
+    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C31" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D31" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="C32" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C33" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C34" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C35" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C36" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C39" s="2"/>
+    </row>
+    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C41" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="E41" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I41" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C42" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="H42" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I42" s="8" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C43" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E43" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="H43" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C44" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D44" s="3">
+        <v>630</v>
+      </c>
+      <c r="E44" s="4">
+        <v>630</v>
+      </c>
+      <c r="H44" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I44" s="8" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C45" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="E45" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="H45" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I45" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="46" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="C46" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="E46" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="F46" s="11" t="s">
+        <v>156</v>
+      </c>
+      <c r="H46" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="C47" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="D47" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E47" s="3"/>
+      <c r="H47" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="49" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="D49" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="E49" s="12" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="51" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H51" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I51" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="52" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H52" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="I52" s="14" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="53" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H53" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="I53" s="7" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="54" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H54" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="I54" s="14" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="55" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H55" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="56" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H56" s="10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H57" s="10" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="61" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="I61" s="6">
+        <v>1</v>
+      </c>
+      <c r="J61" s="6">
+        <v>2</v>
+      </c>
+      <c r="K61" s="6"/>
+      <c r="L61" s="6"/>
+      <c r="M61" s="6">
+        <v>2</v>
+      </c>
+      <c r="N61" s="6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H62" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="I62" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="J62" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="L62" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="M62" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="N62" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="63" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H63" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="I63" s="13" t="s">
+        <v>160</v>
+      </c>
+      <c r="J63" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="L63" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="M63" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="N63" s="15" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="H64" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I64" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="J64" t="s">
+        <v>150</v>
+      </c>
+      <c r="L64" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="M64" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="N64" s="15" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="65" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H65" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="I65" s="7">
+        <v>400</v>
+      </c>
+      <c r="J65">
+        <v>400</v>
+      </c>
+      <c r="L65" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="M65" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="N65" s="15" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="66" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H66" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I66" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="J66" s="13" t="s">
+        <v>159</v>
+      </c>
+      <c r="L66" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="M66" s="13" t="s">
+        <v>155</v>
+      </c>
+      <c r="N66" s="15" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="67" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H67" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="I67" s="13" t="s">
+        <v>152</v>
+      </c>
+      <c r="J67" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="L67" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="M67" s="7"/>
+      <c r="N67" s="16"/>
+    </row>
+    <row r="68" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="H68" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I68" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="L68" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="M68" s="7"/>
+      <c r="N68" s="16"/>
+    </row>
+    <row r="70" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="N70" s="16" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="72" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="L72" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="M72" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="73" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="L73" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C31" t="s">
-        <v>142</v>
-      </c>
-      <c r="D31" t="s">
+      <c r="M73" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="74" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="L74" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C32" t="s">
+      <c r="M74" s="8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="75" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="L75" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="M75" s="8" t="s">
         <v>143</v>
       </c>
-      <c r="D32" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="33" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C33" t="s">
-        <v>144</v>
-      </c>
-      <c r="D33" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="34" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D34" t="s">
+    </row>
+    <row r="76" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="L76" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="M76" s="10" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="77" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="L77" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D35" t="s">
+    <row r="78" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="L78" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="D36" t="s">
+    <row r="79" spans="8:14" x14ac:dyDescent="0.25">
+      <c r="L79" s="6" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="82" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L82" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="M82" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="83" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L83" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="M83" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="84" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L84" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="M84" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="85" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L85" s="17" t="s">
+        <v>2</v>
+      </c>
+      <c r="M85" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="86" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L86" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="M86" s="9"/>
+    </row>
+    <row r="87" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L87" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="M87" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="88" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L88" s="17" t="s">
+        <v>10</v>
+      </c>
+      <c r="M88" s="8" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="89" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L89" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="M89" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="90" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L90" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="M90" s="8" t="s">
+        <v>171</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Search_in_export_CIM = do dokończenia zaraz
</commit_message>
<xml_diff>
--- a/CIM_import_program/powiązania.xlsx
+++ b/CIM_import_program/powiązania.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Programming\Python_Micro_Codes\CIM_import_program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBB571A-2EA8-45E5-A864-4A0A95603BF0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8842C73-17E0-4B62-9D1A-6BEAD6FB0B74}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="53640" yWindow="2280" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="173">
   <si>
     <t>cim:DiscreteValue</t>
   </si>
@@ -518,9 +518,6 @@
     <t>_b8a73c1e5bf443c38cc92c95f1525a54</t>
   </si>
   <si>
-    <t>BYŁO</t>
-  </si>
-  <si>
     <t>_7dcb88942a954fd7befdaa6de1b2216e</t>
   </si>
   <si>
@@ -543,18 +540,32 @@
   </si>
   <si>
     <t>#_fe72415910bf4d1d8edc4573c2b2ea2a</t>
+  </si>
+  <si>
+    <t>Brak tego obiektu "_3e67567dfa9443169ecc1ee28ee67f48"</t>
+  </si>
+  <si>
+    <t>Pojawia się w dużej liczbie stacji</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -592,7 +603,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -614,6 +625,48 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -639,46 +692,85 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -696,6 +788,2335 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1199925</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>73560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>2181885</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>15660</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="6" name="Pismo odręczne 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FEDB8E4-0613-4F1B-9ED9-911281535F09}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6067200" y="1978560"/>
+            <a:ext cx="3420360" cy="4323600"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="6" name="Pismo odręczne 5">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FEDB8E4-0613-4F1B-9ED9-911281535F09}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6058559" y="1969561"/>
+              <a:ext cx="3438002" cy="4341239"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1867005</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>103020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1115205</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>39060</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="9" name="Pismo odręczne 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52DB0BF3-FAD9-405F-8D48-CD85C8C4DC6D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="6734280" y="5627520"/>
+            <a:ext cx="1686600" cy="2984040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="9" name="Pismo odręczne 8">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{52DB0BF3-FAD9-405F-8D48-CD85C8C4DC6D}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="6725640" y="5618520"/>
+              <a:ext cx="1704240" cy="3001680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>28365</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>6540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>1914765</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>23580</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="12" name="Pismo odręczne 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87C392A6-D7DD-4C95-BBDC-19CC2BF4BA20}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7334040" y="5531040"/>
+            <a:ext cx="1886400" cy="3065040"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="12" name="Pismo odręczne 11">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{87C392A6-D7DD-4C95-BBDC-19CC2BF4BA20}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId6"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7325400" y="5522400"/>
+              <a:ext cx="1904040" cy="3082680"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>56805</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>159240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>834915</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>65460</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="15" name="Pismo odręczne 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BFE02F4-B690-4795-8F16-F813162C59F3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7362480" y="5493240"/>
+            <a:ext cx="9331560" cy="2763720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="15" name="Pismo odręczne 14">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7BFE02F4-B690-4795-8F16-F813162C59F3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7353840" y="5484600"/>
+              <a:ext cx="9349200" cy="2781360"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1982280</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>28140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>916920</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>131460</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="21" name="Pismo odręczne 20">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27EEF345-B125-4984-BD67-AF9B2FAFBCB2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="17755680" y="8410140"/>
+            <a:ext cx="1373040" cy="2389320"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="21" name="Pismo odręczne 20">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{27EEF345-B125-4984-BD67-AF9B2FAFBCB2}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId10"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="17746680" y="8401140"/>
+              <a:ext cx="1390680" cy="2406960"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2190270</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>18780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2190630</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>19140</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="47" name="Pismo odręczne 46">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4072889F-BED5-4913-A7A1-DFFF3EABBAD0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14315595" y="11829780"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="47" name="Pismo odręczne 46">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4072889F-BED5-4913-A7A1-DFFF3EABBAD0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14306955" y="11820780"/>
+              <a:ext cx="18000" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1904790</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>85380</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1905150</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>85740</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="48" name="Pismo odręczne 47">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63D17EA0-0682-4BB4-8C93-41ED79FB436B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="14030115" y="11896380"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="48" name="Pismo odręczne 47">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{63D17EA0-0682-4BB4-8C93-41ED79FB436B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="14021475" y="11887380"/>
+              <a:ext cx="18000" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1657110</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>76020</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>1657470</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>85740</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="51" name="Pismo odręczne 50">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB10118-00DA-472A-982A-8797ED9909A5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="13782435" y="11887020"/>
+            <a:ext cx="360" cy="9720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="51" name="Pismo odręczne 50">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0BB10118-00DA-472A-982A-8797ED9909A5}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId15"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="13773795" y="11878020"/>
+              <a:ext cx="18000" cy="27360"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>113925</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>140340</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>1218555</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>59340</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="59" name="Pismo odręczne 58">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{163A2D6D-3B8F-4589-86F2-59C4916DF695}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="7419600" y="7188840"/>
+            <a:ext cx="9658080" cy="2205000"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="59" name="Pismo odręczne 58">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{163A2D6D-3B8F-4589-86F2-59C4916DF695}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId17"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7410960" y="7180200"/>
+              <a:ext cx="9675720" cy="2222640"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>18600</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>85560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>18960</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>85920</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId18">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="60" name="Pismo odręczne 59">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{628EADE1-B2E2-4847-92B4-D4F427181BF3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="18230400" y="10182060"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="60" name="Pismo odręczne 59">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{628EADE1-B2E2-4847-92B4-D4F427181BF3}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="18221760" y="10173060"/>
+              <a:ext cx="18000" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228120</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>113820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>228480</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>114180</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId19">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="61" name="Pismo odręczne 60">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DD86AB1-BA9F-41EA-A675-21594D3FABEC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="18439920" y="8495820"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="61" name="Pismo odręczne 60">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2DD86AB1-BA9F-41EA-A675-21594D3FABEC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId12"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="18431280" y="8486820"/>
+              <a:ext cx="18000" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2224440</xdr:colOff>
+      <xdr:row>51</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>954960</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>152880</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId20">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="62" name="Pismo odręczne 61">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE9637EE-7597-4A7B-BCC1-8862835A39F9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="17997840" y="10191750"/>
+            <a:ext cx="1168920" cy="4629630"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="62" name="Pismo odręczne 61">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AE9637EE-7597-4A7B-BCC1-8862835A39F9}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId21"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="17988840" y="10182750"/>
+              <a:ext cx="1186560" cy="4647270"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2165760</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>84540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2390400</xdr:colOff>
+      <xdr:row>76</xdr:row>
+      <xdr:rowOff>15660</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId22">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="63" name="Pismo odręczne 62">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C030F40-9B6F-4E04-B518-4A790EE20BBB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="17939160" y="14562540"/>
+            <a:ext cx="224640" cy="312120"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="63" name="Pismo odręczne 62">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4C030F40-9B6F-4E04-B518-4A790EE20BBB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId23"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="17930520" y="14553900"/>
+              <a:ext cx="242280" cy="329760"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>3480</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>46920</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>486600</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>96180</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId24">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="66" name="Pismo odręczne 65">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D1EBA30-09E3-4805-81C4-9646FC627E98}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="18215280" y="10524420"/>
+            <a:ext cx="483120" cy="1382760"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="66" name="Pismo odręczne 65">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9D1EBA30-09E3-4805-81C4-9646FC627E98}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId25"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="18206640" y="10515778"/>
+              <a:ext cx="500760" cy="1400405"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>142440</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>113880</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>154680</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>84660</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId26">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="78" name="Pismo odręczne 77">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB324DF3-D95B-4468-BAD7-96EBE72F4408}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="18354240" y="11734380"/>
+            <a:ext cx="12240" cy="161280"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="78" name="Pismo odręczne 77">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB324DF3-D95B-4468-BAD7-96EBE72F4408}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId27"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="18345600" y="11725380"/>
+              <a:ext cx="29880" cy="178920"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2037960</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>28140</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>400560</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>147960</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId28">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="81" name="Pismo odręczne 80">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA5AD5D1-94E1-4ABA-AFA4-3A7E56252A6F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="17811360" y="11839140"/>
+            <a:ext cx="801000" cy="2596320"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="81" name="Pismo odręczne 80">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA5AD5D1-94E1-4ABA-AFA4-3A7E56252A6F}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId29"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="17802724" y="11830140"/>
+              <a:ext cx="818632" cy="2613960"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>342600</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>75960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1047840</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>32340</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId30">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="84" name="Pismo odręczne 83">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E15A5FC-B416-484F-A4CD-548B4D89F11E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="18554400" y="12077460"/>
+            <a:ext cx="705240" cy="2432880"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="84" name="Pismo odręczne 83">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8E15A5FC-B416-484F-A4CD-548B4D89F11E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId31"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="18545760" y="12068460"/>
+              <a:ext cx="722880" cy="2450520"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>875760</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>189420</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1046040</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>29160</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId32">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="85" name="Pismo odręczne 84">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1880FA2F-385E-47DA-9A2D-BC25240FC9F0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="19087560" y="14286420"/>
+            <a:ext cx="170280" cy="30240"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="85" name="Pismo odręczne 84">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1880FA2F-385E-47DA-9A2D-BC25240FC9F0}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId33"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19078920" y="14277420"/>
+              <a:ext cx="187920" cy="47880"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>897720</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>171420</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1034160</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>152640</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId34">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="86" name="Pismo odręczne 85">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B18E7AF-B0C0-4F07-92D5-29B90CE5D59B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="19109520" y="14268420"/>
+            <a:ext cx="136440" cy="171720"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="86" name="Pismo odręczne 85">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2B18E7AF-B0C0-4F07-92D5-29B90CE5D59B}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId35"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19100880" y="14259780"/>
+              <a:ext cx="154080" cy="189360"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>869640</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>150540</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>1047840</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>117000</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId36">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="89" name="Pismo odręczne 88">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98217A3-13BD-4C71-80F3-B2936AEA32EC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="19081440" y="14247540"/>
+            <a:ext cx="178200" cy="156960"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="89" name="Pismo odręczne 88">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B98217A3-13BD-4C71-80F3-B2936AEA32EC}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId37"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="19072440" y="14238900"/>
+              <a:ext cx="195840" cy="174600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2018880</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>142620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2160720</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>360</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId38">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="92" name="Pismo odręczne 91">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA1AEC4E-EED7-4418-A0E6-B7C5AE26197C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="17792280" y="14239620"/>
+            <a:ext cx="141840" cy="48240"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="92" name="Pismo odręczne 91">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA1AEC4E-EED7-4418-A0E6-B7C5AE26197C}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId39"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="17783640" y="14230620"/>
+              <a:ext cx="159480" cy="65880"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2046600</xdr:colOff>
+      <xdr:row>72</xdr:row>
+      <xdr:rowOff>147660</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>2136240</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>125280</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId40">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="93" name="Pismo odręczne 92">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13A13AFE-89BB-44CA-B0B8-3AB8CC197341}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="17820000" y="14244660"/>
+            <a:ext cx="89640" cy="168120"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="93" name="Pismo odręczne 92">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{13A13AFE-89BB-44CA-B0B8-3AB8CC197341}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId41"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="17811000" y="14236020"/>
+              <a:ext cx="107280" cy="185760"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>33360</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>136560</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>146400</xdr:colOff>
+      <xdr:row>60</xdr:row>
+      <xdr:rowOff>58020</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId42">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="96" name="Pismo odręczne 95">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37910140-2FFB-4137-921E-D9C26E208D36}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="18245160" y="11757060"/>
+            <a:ext cx="113040" cy="111960"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="96" name="Pismo odręczne 95">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{37910140-2FFB-4137-921E-D9C26E208D36}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId43"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="18236520" y="11748420"/>
+              <a:ext cx="130680" cy="129600"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>94950</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>85500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>95310</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>85860</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId44">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="97" name="Pismo odręczne 96">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32922B6D-D57C-465B-9A43-D8B245964FDB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="18840150" y="12468000"/>
+            <a:ext cx="360" cy="360"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="97" name="Pismo odręczne 96">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32922B6D-D57C-465B-9A43-D8B245964FDB}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId45"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="18831510" y="12459000"/>
+              <a:ext cx="18000" cy="18000"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>28350</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>190320</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>533670</xdr:colOff>
+      <xdr:row>80</xdr:row>
+      <xdr:rowOff>162240</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:xdr14="http://schemas.microsoft.com/office/excel/2010/spreadsheetDrawing" Requires="xdr14">
+        <xdr:contentPart xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId46">
+          <xdr14:nvContentPartPr>
+            <xdr14:cNvPr id="119" name="Pismo odręczne 118">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5479BCEC-4052-4D00-A8A4-396488848B68}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr14:cNvPr>
+            <xdr14:cNvContentPartPr/>
+          </xdr14:nvContentPartPr>
+          <xdr14:nvPr macro=""/>
+          <xdr14:xfrm>
+            <a:off x="18773550" y="12382320"/>
+            <a:ext cx="2943720" cy="3400920"/>
+          </xdr14:xfrm>
+        </xdr:contentPart>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:pic>
+          <xdr:nvPicPr>
+            <xdr:cNvPr id="119" name="Pismo odręczne 118">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5479BCEC-4052-4D00-A8A4-396488848B68}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvPicPr/>
+          </xdr:nvPicPr>
+          <xdr:blipFill>
+            <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId47"/>
+            <a:stretch>
+              <a:fillRect/>
+            </a:stretch>
+          </xdr:blipFill>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="18764910" y="12373320"/>
+              <a:ext cx="2961360" cy="3418560"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+          </xdr:spPr>
+        </xdr:pic>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/ink/ink1.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T08:24:39.724"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#E71224"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">3599 33,'51'1,"-13"0,0-1,0-2,0-2,35-8,-31 5,0 2,-1 2,1 1,1 3,10 2,44-1,856-2,-923 2,-1 1,0 1,1 1,1 1,1-2,14 0,8 0,44 9,-28-3,-4 2,-46-7,1-1,-1-2,12 1,-7-1,1 1,25 7,6 1,102 22,-78-14,-69-16,0 1,1 0,-2 1,1 1,-1 0,1 0,-2 1,1 0,-1 1,0 1,18 11,-19-13,20 14,0 1,21 22,-35-31,0-1,1-1,1 0,0-1,7 2,18 12,245 165,-242-157,0 2,-3 2,14 17,54 63,3 13,-1 7,16 27,-48-64,131 173,-158-203,4 11,34 46,-68-97,90 122,13 46,-10-32,-84-113,-2 2,2 13,3 2,119 211,-85-144,-42-79,33 52,-45-84,-2 1,-1 1,5 16,18 41,41 93,-46-104,13 43,-6 2,6 44,13 75,-45-188,-6-31,-1 0,-1 0,1 14,12 88,-6-56,2 2,-6-35,-2 0,1 27,-2-21,1 0,5 14,1 9,1 5,-5-34,-1 0,0 27,-3-34,1-1,5 22,-3-21,-1-1,0 23,-5 72,-1-58,5 53,23 20,-16-45,20 85,-16-102,-2 1,-4 0,-1 34,-8 1614,-1-1700,0 0,0 0,-6 14,4-12,0 0,1 0,1 2,0-3,-1-1,-1 0,-1 0,-1 0,-1 0,-1 1,-15 49,8-15,-3-1,-3-1,-1 0,-3-2,-12 15,-64 122,27-46,27-68,-3-3,-40 43,32-41,-1-4,-4-3,-32 25,-5 5,-63 42,135-112,-1-2,-8 4,5-4,-14 11,-1-2,-1-2,-2-3,-2-1,-48 23,17-9,-58 20,98-44,0 1,-35 21,61-30,-1-2,1 0,-2-2,1 1,-5-1,-45 14,43-12,0-1,-21 3,-11 2,-8 5,0 2,1 4,-41 20,22-7,39-18,1 2,-7 7,22-13,0-1,0 0,-18 2,-54 23,61-22,-1-1,-1-3,-4 0,6-1,-203 63,70-20,-181 58,221-83,128-27,-81 17,-27 0,-21 7,74-14,32-5,0-2,0 0,-18-1,14-4,-1 2,1 2,0 0,-14 5,18-3,-1-1,1-2,-9 0,16-2,0 1,1 1,-1 1,0 0,1 2,0 0,-4 2,-5 3,0-2,0-1,0-1,-2-1,-6 2,0 0,-6 5,7-1,-27 9,-56 26,80-30,-40 11,47-18,1 2,1 0,0 2,-3 3,16-8,0-1,0 0,-1-2,-7 2,-42 15,50-16,-1-1,0 0,0-1,-13 0,11-1,1 0,0 1,-1 1,-2 2,-235 81,232-81,0-1,0-1,0-1,-32 7,-77 15,104-21,0-1,0-2,-28-1,29-1,-1 2,1 0,-1 2,-5 2,-11 1,0-2,0-1,0-3,0-1,-10-4,-52 1,57 4,12 0,0-1,0-2,0-2,-35-8,-84-15,128 22,0 1,1 2,-16 1,16 0,0-1,0 0,-24-7,-133-18,0 0,156 22,0 1,-20 0,19 2,0-1,-15-5,-86-19,-28 1,27 0,114 21</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1202.27">583 11436,'-121'-2,"30"0,-69 7,137-1,1 0,-1 2,2 0,-1 1,0 2,2 0,-1 1,-1 2,21-11,0-1,0 1,0-1,0 1,0 0,1-1,-1 1,0 0,0 0,1-1,-1 1,0 0,1 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,1-1,-1 0,0 0,1 0,-1 0,1-1,-1 1,1 0,-1 0,1 0,0 0,-1 0,1-1,0 1,0 0,46 44,-33-33,25 23,33 35,-59-58,0 0,1 0,1-1,-1-1,2 0,-1-1,4 0,19 13,-16-11,0-2,1 0,0-1,0-1,23 4,56 17,1 4,-60-20,-1 2,9 6,-39-16,-1 0,1-1,0-1,-1 0,1 0,5-1,51 11,-50-7</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2939.17">874 86,'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink10.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:18:06.571"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#66CC00"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink11.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:18:17.345"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#66CC00"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink12.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:18:24.662"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#66CC00"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">700 0,'8'1,"1"-1,-1 1,1 1,-1-1,8 3,31 4,113 13,-137-17,-1 1,-1 0,1 0,-1 2,14 5,49 14,-68-20,1 0,-1 0,0 1,-1 1,-1-1,1 2,3 3,40 21,74 43,-122-71,-2 1,1 0,-1 1,-1-1,1 1,1 4,28 23,-5-8,-1 0,11 17,-3-4,-3-3,17 24,52 68,-65-79,9 11,-25-25,2 0,19 17,15 27,-47-59,1 0,1-1,2 0,17 15,-3-5,-1 1,-3 1,17 27,-17-21,-14-17,1-1,2 0,0-1,6 4,-3-4,-2 1,-1 0,8 14,17 20,-27-34,-1 0,-1 0,-1 3,-3-7,0 0,2 0,0-1,1 0,12 12,-15-17,0 0,-2 1,0-1,0 1,-1 1,-1-1,0 0,-1 1,0 6,14 34,41 77,-30-51,-15-35,19 32,19 57,-33-93,-3 0,1 12,-3-10,13 73,-8-56,1 29,-7-36,-6-31,-2 0,-1 0,-1 6,0 3,2 1,3 6,-1-8,-2 1,-1 13,-3-23,1-1,1 1,1-1,6 15,-3-10,-2 0,-2 0,0 1,-3 11,1-11,0-1,3 1,0-1,4 10,1 1,-3-1,-2 1,-2 0,-1 0,-3 2,0 41,3 282,-1-344,-1 0,-1 1,-5 9,4-8,0-1,1 1,1 1,1 4,-1 0,-1-1,-7 20,-17 91,23-118,-12 41,-2 22,13-57,-1-1,0 0,-2 0,-6 7,6-10,0 1,2 0,0-1,1 2,-1 13,4-17,-1-1,-1 0,0 0,-1 0,-6 7,-12 34,0 8,15-46,2 1,0 0,2 0,0 1,0 11,2-7,-2 1,-1-1,-1 0,-3 4,1-5,2 1,1-1,1 1,0 12,3-9,-2 0,-5 14,2-14,2 0,1 12,1-21,0 0,-1 0,-4 7,3-6,0 0,1 0,1 1,0 494,5-249,-3 547,-2-790,0 0,-2 0,-2 2,1 0,1-1,0 12,0-6,-1 0,-2 1,-1-2,-4 4,0 6,0-5,7-19,0 0,2 1,0 0,-1 8,0 9,-3-1,-1 1,-12 25,5-15,-5 26,2 2,-6 4,3-7,-1 16,17-60,-2 0,-9 16,-7 21,5-8,-25 43,1-5,5-10,-44 62,31-61,45-71,1 0,0 1,0-1,1 1,1 0,0 0,0 0,1 0,-2 1,0 0,0 0,-1-1,-3 5,3-7,-26 37,2 2,-6 19,20-32,-17 35,-22 47,47-103,1 1,0 0,1 0,0 4,1-2,-1 0,-1 0,-3 3,-7 12,2 1,2-1,-5 30,10-39,-1 0,-1 0,-9 13,-14 32,18-33,7-20,1 0,1 0,1 0,0 1,1 0,-1 3,-1 0,-1 1,-1-2,-1 1,-1 0,-1-1,-4 5,-1 0,3 1,0 0,-2 13,3-4,-1 0,-2-1,-15 25,-26 59,-52 75,74-129,22-40,0 0,-2 0,-1-1,-5 6,1-4,2 0,-7 15,9-13,-2-1,-10 11,15-18,1-1,0 1,1 0,1 0,-1 3,-1-1,-11 14,-65 97,12-28,62-85,2 0,-1 1,-4 13,8-16,0 0,-2 0,0 0,0 0,-2-1,-1 1,1-1,1 0,1 0,0 0,1 1,1 0,-3 8,3-7,0 0,-2 0,0 0,-1 0,-4 3,5-7,1 1,0 1,1-1,1 1,0-1,1 2,-20 37,-55 102,63-122,1 1,-4 19,-7 15,-14 1,14-27,-8 31,25-49,-1 0,-1 0,-12 15,10-17,2-1,-4 13,-8 11,10-21,0 2,-1-1,-16 18,20-26,0 0,1 1,1 0,0 3,3-5,-2 0,0-1,-1 1,0-1,-1 0,-3 2,0 0,2-1,0 1,1 0,1 1,-3 8,-20 30,3-13,14-21,1 0,1 0,1 1,1 0,-1 9,11-27,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,-1 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1-1,0 1,0 0,0 0,-1 0,1-2,0 1,0 0,0-1,0 1,1-1,-1 1,0-1,0 1,1-1,-1 0,0 1,1-1,-1 1,1-1,-1 0,1 0,0 1,-1-1,1 0,0 1,0-1,0 0,-1 0,1 1,0-2,-5-11,-2 1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink13.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:18:31.692"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#66CC00"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">69 108,'1'1,"0"-1,0 0,0 1,0-1,-1 1,1-1,0 1,0-1,0 1,0-1,0 1,-1 0,1 0,0-1,-1 1,1 0,0 0,-1 0,1 0,-1-1,0 1,1 0,-1 0,0 0,1 0,-1 0,9 35,-5-19,2 4,-2 0,0 1,-1-1,-1 1,0 12,1 18,9 21,-7-53,-2 0,0 1,-1 5,-4 52,1-50,0 0,2 0,2 12,-3-40,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,1 1,-1-1,0 0,0 0,0 0,0 1,0-1,1 0,-1 0,0 0,0 1,0-1,1 0,-1 0,0 0,0 0,0 0,1 1,-1-1,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0-1,0 1,14-15,6-24,15-31,3 1,16-18,-30 54,2 1,20-19,-3 10,-28 28,-2-1,1 0,-2-1,7-9,-13 15,-6 11,-16 15,13-14,-1-1,0 0,0 0,0 0,0 0,0 0,0-1,0 0,-1 0,1 0,0 0,-1-1,1 0,-1 0,1 0,-1 0,1-1,0 0,-1 1,1-2,0 1,-2-1,-13-5,1-1,0-1,0-1,-8-6,9 6,-33-21,7 5,-31-14,42 22,1 0,1-2,-15-14,76 56,-20-16,-1 0,-1 1,1 0,-1 0,0 1,-1 1,1 0,-2 0,1 0,-2 1,1 0,4 10,2 15,-2 2,-2-1,-1 1,-1 1,-3 0,-1-1,-1 34,-1-77,1 1,0-1,0 1,1-1,-1 1,1 0,0 0,3-4,41-55,-30 40,116-134,-131 156,4-9,2 1,0 0,0 0,1 0,0 1,0 0,1 1,5-3,-15 11,0 0,0 0,0-1,0 1,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 1,-1-1,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,-6 14,-10 12,5-12,0 1,2 1,0 0,0 0,0 5,2-6,0 0,-1 0,-1-1,0 0,0 0,-7 6,7-9,0 1,1 0,1 0,0 1,1 0,0 0,1 1,1-1,0 1,0 2,-22 63,25-76,-1 0,1 0,-1 0,1 0,-1 0,0 0,0 0,-1-1,1 1,-1-1,3-2,0 1,0-1,-1 0,1 0,0 0,-1 0,1 0,0 1,-1-1,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,-1-1,1 1,0 0,-1 0,1 0,0 0,-1 0,1-1,0 1,0 0,-1 0,1-1,0 1,-9-23,4-12,2-1,2 0,1 0,3-10,-1-20,-2 430,1-398,2 1,2 0,1-5,0 9,5-33,-3 24,-2 1,-1-2,-2-7,-19 164,3-35,-12 40,69-173,-42 48,12-20,0 1,2 1,10-10,-20 25,-1-1,2 1,-1 0,0 0,1 1,0 0,0 0,0 0,1 1,-1 0,1 1,0 0,3-1,2 1,-1-1,1 0,-1-1,0-1,0 0,5-3,-31 16,1 1,0 1,1 0,0 1,1 0,0 0,1 2,-1 0,1-1,0-1,-1-1,-1 0,0 0,-7 4,-35 30,9-3,25-23,0 0,2 2,-7 9,69-89,-9 9,3 3,27-27,-54 62,1-1,-2 0,0-1,4-8,-8 11,1 1,0 0,1 1,0-1,0 1,1 1,1 0,9-8,-8 10,43-26,-50 31,-1 0,1 1,0 0,0 0,0 0,0 0,-1 1,1-1,0 1,0 0,0 0,0 1,0-1,2 2,-5-2,-1 0,0 0,1 0,-1 0,0 0,0 1,1-1,-1 0,0 0,0 1,1-1,-1 0,0 0,0 1,0-1,1 0,-1 1,0-1,0 0,0 0,0 1,0-1,0 0,0 1,1-1,-1 0,0 1,0-1,0 0,0 1,-1-1,1 0,0 1,0-1,0 0,0 1,0-1,0 0,0 1,-1-1,1 0,0 0,0 1,0-1,-1 0,1 0,0 1,0-1,-1 0,1 0,0 0,-1 1,1-1,0 0,0 0,-1 0,1 0,0 0,-1 0,1 0,-30 24,4-3,-10 18,23-25,-1 0,2 1,0 1,1 0,1 0,-4 8,5-6,-1 0,-1-1,0-1,-1 0,-1 0,0-1,-7 5,-21 28,31-36,0 1,-1-1,0-1,-6 4,4-2,0 0,1 1,0 0,1 1,-4 9,-14 16,16-17,10-18,11-14,20-37,-19 30</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink14.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:19:53.791"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#AB008B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">96 1,'29'0,"0"0,1 2,-1 1,0 1,0 1,-1 2,25 9,17 6,20 8,18 20,-64-28,-33-17,0 0,-1 0,0 1,0 0,0 1,3 4,27 23,-23-20,0 0,-2 1,0 1,4 5,15 22,-5-6,0 2,3 10,-27-41,1 0,1 0,-1-1,2 0,-1 0,1 0,34 37,3 21,-2 2,11 30,-40-66,-1 1,-2 1,0 0,-3 0,0 4,15 72,-11-55,-1 0,1 42,-11 205,-2-152,0-133,-1 0,0 0,-1 0,-3 5,-7 53,-3 27,5-44,-15 57,-1 10,17-59,-3 0,-2-2,-4 5,-2-24,17-37,0 1,0-1,1 1,0 0,0 0,1 0,-1 5,-3 14,-1 0,-1-1,-1 0,-2-1,0 0,-2 0,-1-2,-15 22,24-37,-32 61,28-49,-1-1,-1 0,-1 0,-4 5,1-4,2 0,1 1,-10 22,10-19,0-1,-2 0,-4 3,-10 12,-71 89,86-113,-2-1,1-1,-1 0,-1-1,0 0,-1-1,0-1,0-1,-1 0,0-1,-1-1,1-1,-7 0,-14 4,0-2,0-1,-1-3,-13 0,31-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="2050.96">467 3361,'-14'1,"1"0,-1 1,1 0,0 1,0 1,0 0,0 1,1 0,0 1,0 0,0 1,1 0,0 1,0 0,1 1,0 0,-4 4,-10 8,-1-2,-1 0,-1-2,-8 3,-49 33,83-52,-1 0,0 0,1 0,-1 1,1-1,-1 0,1 1,0-1,-1 1,1-1,0 1,0 0,0 0,0-1,0 1,1 0,-1 0,0 0,1 0,-1 0,1 0,0 0,0 0,0 1,0 0,1-1,0 1,0-1,0 1,0-1,1 1,-1-1,1 0,-1 0,1 1,0-1,0 0,-1 0,2-1,-1 1,0 0,6 4,0-1,0 0,1-1,-1 1,1-1,0-1,0 0,0 0,0-1,2 0,1 0,0 1,-1 0,1 0,-1 1,0 0,6 4,16 6,-20-10,0 0,1-1,-1-1,13 1,-14-2,0 1,0 0,0 0,-1 1,1 0,-1 1,1 1,-1 0,0 0,0-1,0-1,0 0,0 0,1-1,-1 0,4-1,7 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink15.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:20:35.998"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#AB008B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'21'57,"-15"-6,-2 1,-2 0,-3 0,-2 2,1 53,2-84</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink16.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:20:41.465"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#AB008B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1509 0,'12'2,"1"0,-1 0,0 1,0 0,0 1,0 1,-1 0,1 1,-1 0,-1 0,1 1,1 2,1 1,0-2,0 1,1-2,2 1,16 9,-26-13,-1 0,0 0,-1 0,1 1,-1 0,0-1,0 1,2 4,28 29,-26-31,-1-1,0 1,0 0,0 1,-1 0,-1 0,1 0,-1 0,1 3,33 85,-30-70,1 1,1-2,2 0,0 1,-1 1,-1 0,-2 0,2 11,-2-9,19 48,-15-45,-2 0,4 24,12 30,-19-65,-1 2,-1-1,1 10,4 23,-6-32,-1 1,-1 0,0 9,-2-11,2 1,0-1,3 4,-1-3,-1 0,-2 0,0 1,-1 410,-2-206,0-212,-1 0,0 0,-1 0,-3 5,-7 53,11-53,-2 0,-1 0,0 0,-6 12,5-13,0 0,1 1,1 0,-2 17,4-17,-2 0,0 0,-1 0,-6 14,4-15,1 1,1 0,1 0,-1 15,0 13,-3-1,-2 0,-2-1,-3 0,-8 19,-26 88,43-133,0 4,-1 1,-1-1,-2 0,0-1,-5 7,-37 78,37-73,-2 0,-11 15,7-17,-32 50,4 3,3 5,8 0,25-56,-1-2,-2 1,-2-2,-1 0,-1-1,2-4,1 1,1 1,1 0,-8 29,-26 51,-21 31,53-108,0 0,-12 15,13-23,1 0,2 1,0 0,-4 18,11-30,0 0,-1-1,0 0,-1 0,-7 9,5-9,1 2,1-1,0 1,-3 9,1-1,-2-1,0 0,-1 0,-10 10,10-13,0 0,1 0,1 1,1 1,-5 13,2-1,-1 0,-3-1,0-1,-2-1,-2 2,-7 10,2 2,1 2,-4 17,5-11,-1 0,-21 27,-56 83,84-128,2 0,1 1,-9 35,12-36,-2 7,-2 0,-2-1,-2-1,-12 17,29-49,-1 0,1 1,0-1,1 1,0 0,0 0,1 0,-1 3,1-3,0 0,-1 0,0 0,0 0,-1 0,0 0,-4 7,-7 13,0 0,2 1,1 1,1 0,2 1,1-1,-2 23,5-30,-2 0,-1 0,-1-1,-5 10,5-14,1 0,0 0,2 1,0 0,1 0,0 11,3-8</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1547.85">1 6827,'1'1,"1"0,0 0,-1-1,1 1,0 0,-1 0,1 0,-1 1,0-1,1 0,-1 0,0 1,0-1,0 1,0-1,0 1,0 0,0 1,16 32,-7-2,-2 0,-1 1,-2 0,-1 0,-1 0,-2 22,-1-51,0-1,0 1,1-1,0 1,0-1,0 1,0-1,1 0,-1 0,1 1,0-1,2 1,-4-4,1 0,-1-1,1 1,-1-1,1 1,-1-1,1 1,-1-1,1 1,0-1,-1 1,1-1,0 0,-1 1,1-1,0 0,0 0,-1 0,1 1,0-1,0 0,-1 0,1 0,0 0,0 0,-1 0,1-1,1 0,0 0,0 0,0 0,0 0,-1 0,1-1,0 1,-1-1,1 1,-1-1,0 0,0 1,1-1,-1 0,0-1,35-74,-31 63,1 1,0-1,1 1,0 0,1 1,1 0,6-7,87-107,-78 99,-11 16</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink17.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:20:47.544"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#AB008B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'2'1,"0"0,1-1,-1 1,0 0,0 0,1 0,-1 0,0 0,0 1,0-1,-1 1,1-1,0 1,0 0,-1 0,1 0,-1 0,0 0,2 1,24 47,-23-42,62 115,27 48,5-4,-67-90,-22-52,1-1,10 18,-8-16,-1 1,0 1,-2-1,-2 2,1 3,23 80,0-12,-20-62,0-1,14 27,81 200,-56-155,-36-82,-2 0,-1 0,3 15,18 44,47 126,-54-155,10 37,-17-31,-5-20,1 0,13 27,-15-39,-1 0,-2 1,6 32,-8-32,0-1,3 1,0-2,6 8,-5-9,-1 0,0 0,-3 1,0 0,0 1,1 0,1 0,10 17,-10-24,-1 0,-1 0,1 7,15 49,-11-44,-1 1,-2-1,2 24,16 47,-1-2,27 106,-27-77,0 23,-17-111,12 37,1 2,-13-46,-2 0,-1 0,-3 0,0 15,-1-15,1 0,7 29,2 24,14 94,-15-106,-4-37,-2 0,-1 29,-4-47,1 0,1 0,1 0,5 18,0 3,-3 0,-2 0,-2 1,-1-1,-4 3,2 57,2-83,-1 11,2 1,1-1,1 1,8 26,16 97,0-26,0 0,-7-54,26 58,-94-176,35 28</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1243.28">1456 6165,'4'2,"0"-1,0 1,0 0,0 0,0 0,-1 0,1 1,-1 0,1-1,1 4,13 7,75 53,-45-29,-34-25,0 1,-1 0,-1 1,0 0,5 10,12 13,-21-25,0-1,-1 1,-1 0,0 1,0 2,17 31,56 87,-74-124,0 1,-1-1,0 1,-1 0,0 0,0 0,-11-31,3 10,0 0,1 0,1-1,-2-9,0-44,3-1,4-27,0-4,-1 76,2 0,0 1,1-1,1 1,5-13,-2 8,-1-1,-2 1,0-2,-3 6</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink18.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:20:59.164"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#AB008B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 2,'30'0,"-16"-1,0 0,1 1,-1 1,0 0,0 1,0 1,0 0,0 1,-1 0,1 1,10 6,-3-2,-1-1,2-1,-1 0,1-2,0 0,0-2,0 0,0-1,0-2,3 0,-2 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink19.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:21:06.873"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#AB008B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">46 105,'0'1,"0"0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1-1,0 1,-1 0,1 0,0-1,0 1,-1 0,1-1,0 1,0-1,0 1,0-1,0 1,0-1,0 0,0 1,1-1,33 9,-17-5,31 17,17 6,-61-26,-1 1,0 0,0 1,0-1,0 1,0-1,0 1,-1 0,1 1,-1-1,0 1,0-1,0 1,-1 0,1 0,-1 0,0 0,0 1,0 1,-1-4,0 0,0 0,-1-1,1 1,0 0,-1 0,0 0,0 0,1 0,-1 0,0 0,-1 0,1 0,0 0,0 0,-1 0,0 0,1 0,-1 0,0 0,0 0,0-1,0 1,0 0,0-1,0 1,0-1,-1 1,1-1,-1 1,1-1,-1 0,0 0,1 0,-1 0,0 0,0 0,0 0,0-1,0 1,1-1,-1 1,0-1,-2 0,-2 1,-1 0,1-1,0 0,-1-1,1 1,0-1,-2 0,6 0,0 1,0 0,0-1,0 1,0-1,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,1-1,-1 1,1-1,-1 1,1-1,0 0,0 1,-1-1,1-2,1 1,1-1,-1 1,1 0,0-1,0 1,1 0,-1 0,1 0,0 0,-1 0,1 0,1 0,-1 0,0 1,1-1,0 0,10-13,42-94,-51 103,-1 0,0-1,-1 0,0 0,1-5,-2 7,0 0,0 0,1 0,0 0,0 0,1 1,-1-1,1 1,1-1,0 11,-1 0,0 0,0 1,0 0,0-1,-1 1,0 0,1 5,0 11,0 1,-1 0,-2 0,0 0,-2 5,1-6,0 0,2 0,0 1,1-1,4 10,12 6,-16-35,1 1,-1 0,0 0,0 0,0 0,-1 0,0 0,1 0,-1 1,0 1,-1-6,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 0,0 1,0-1,0 0,-1 0,1 1,0-1,0 0,0 0,0 0,0 1,-1-1,1 0,0 0,0 0,0 1,-1-1,1 0,0 0,0 0,-1 0,1 0,0 1,0-1,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,-19-11,-13-16,20 14,1 0,1-1,-7-11,-23-30,80 109,-36-48,0 0,0 0,0 1,-1-1,0 1,-1 0,1 0,-1 0,0 1,-3-7,1-1,0 1,0 0,-1 0,1-1,-1 1,1 0,0-1,-1 1,1 0,-1-1,0 1,1-1,-1 1,1-1,-1 1,0-1,1 1,-1-1,0 0,0 1,1-1,-1 0,0 0,0 0,1 1,-1-1,0 0,0 0,0 0,1 0,-1 0,0 0,0-1,0 1,1 0,-1 0,0 0,0-1,0 1,-33-11,24 5,1-1,0-1,1 1,0-1,0-1,-1-2,0 1,0 1,0-1,-1 2,-8-6,14 11,1 0,-1 0,0 0,1 0,0-1,0 1,0-1,0 0,1 0,-1 0,1 0,0 0,0-1,0 1,1-1,-1 0,-11-29,10 29,0 1,-1-1,1 0,-1 1,0 0,0 0,0 0,0 1,-1-1,1 1,-1 0,0 0,-1 0,0-1,13 5,11 9,81 85,-85-80,-1 1,0 1,-1 0,-1 0,6 15,10 13,15 33,-81-127,23 25,-1-1,1 0,1-1,1-1,1-1,-2-11,6 20,0 0,0 1,-2 0,-1 0,0 1,-1 1,0 0,-4-2,5 7</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink2.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T08:25:57.829"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#F6630D"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1614 4,'111'-2,"-23"0,57 7,-12 21,-78-16,-28-4,0-1,0-2,21 1,-14-2,0 2,0 1,0 2,22 7,19 4,-33-7,-24-6,0-1,-1-1,19 2,-12-3,0 1,0 2,0 0,-1 2,12 5,24 11,28 16,98 68,0-1,-120-71,-1 3,42 34,46 30,-93-56,-51-38,0 0,1-1,1 0,-1 0,1-1,0 0,4 1,0-1,-2 1,1 1,-1 0,0 0,0 2,-1-1,-1 1,8 9,-5-5,2 0,0-1,0-1,5 2,8 7,-1 0,0 3,3 5,-14-14,64 51,-48-41,-1 1,-1 2,15 20,-25-25,1-1,1-1,1-1,21 15,-38-31,-1 0,0 1,0 0,0 0,-1 0,1 1,-1-1,0 1,-1 0,0 0,0 1,1 3,27 87,-18-51,-7-23,-1 0,-2 1,0-1,-1 1,-2 22,3 33,10-5,-9-55,0 0,-1 1,-1 8,-2-20,2 44,-5 37,2-72,-2 0,0 0,-1-1,0 1,-1-1,-1 0,-2 2,-46 140,29-96,14-32,-1-1,-10 17,-37 81,-15 37,-23 4,93-161,0-1,0 0,-1 0,0-1,0 1,0-1,-4 3,4-4,0 1,0 0,0 0,0 0,1 1,0 0,0 0,-2 4,-7 15,-1 0,-1-2,-2 0,0 0,-7 5,-8 11,-7 11,12-14,-2-1,-6 5,-45 65,32-43,-9 9,-13 11,19-20,33-43,-2-1,-1 0,-11 6,-48 43,72-59,-32 33,-2-2,-1-2,-5 1,-85 68,79-62,39-31,0 0,-1-1,0-1,-1-1,-1 0,1 0,0 1,1 0,0 1,-11 11,12-10,0-1,-1 0,-1-1,-12 6,9-5,1 0,0 1,1 1,-16 15,13-10,-2 0,-20 11,32-23,-28 17,-2-2,-3 1,33-18,1 1,0 1,0 0,0 0,1 1,0 0,1 0,0-1,-1 0,0 0,-1-1,1 0,-9 3,-15 6,0 1,2 1,0 2,1 1,0 2,-11 12,20-16,-79 67,-2 11,59-62,35-29,1 1,-1 0,1 0,0 0,1 1,-1 0,0 2,-40 51,32-43,0 1,2 0,0 1,-7 16,11-18,-2-1,0 1,0-2,-13 13,11-13,0 0,2 1,0 0,-7 15,-6 12,-2-2,-16 20,9-13,19-29,-18 30,-28 52,49-82,0 0,-2-1,-8 9,7-10,2 0,0 1,-7 14,-36 64,37-67,1 0,2 1,1 0,-4 15,10-23,-1-1,-1 0,-1-1,0 0,-2 0,2 0,1 0,1 0,-1 6,4-9,-1 0,0-1,-1 0,-1 0,-9 12,0-3,2 2,0 0,2 0,1 2,2 0,-7 13,-20 32,-41 85,-134 158,186-265,22-41,-1 1,0-1,0 0,-1 0,-1-1,0 0,-1 1,2-3,0 1,1 0,0 0,0 1,1 0,-1 2,2-3,-1 1,0-2,0 1,-1 0,0-1,-1 0,-2 2,-3 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1173.26">291 7465,'0'27,"-2"0,0 0,-2 0,0 0,-2-1,-1 0,-1 0,-2 0,-10 19,-20 79,-23-7,52-96,1 1,-7 21,-18 36,29-68,-1 0,1-1,0 1,1 0,0 0,1 0,0 1,1-1,-2 13,5-24,0 1,0-1,0 1,0-1,0 0,0 1,0-1,0 1,0-1,1 0,-1 1,0-1,0 0,0 1,0-1,1 1,-1-1,0 0,0 1,1-1,-1 0,0 0,1 1,-1-1,0 0,1 0,-1 1,0-1,1 0,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 1,-1-1,0 0,1 0,22-5,19-15,20-19,-25 16,35-17,-44 26,0-1,-2-1,0-1,-1-1,18-17,-29 24,0 0,1 2,1 0,10-5,-7 5,-2 0,1-2,7-7,22-14,14-13,-1-1,5-5,-48 36,-3 3</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink20.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:21:12.895"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#AB008B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">98 31,'19'-1,"0"-1,0 0,18-6,-16 3,0 1,0 1,6 1,70 2,-127-1,-63-1,-40 6,125-3,1 0,-1 0,1 1,0-1,-1 2,1-1,0 1,0 0,0 1,1-1,-1 1,1 1,-1 0,5-3,0 0,-1 0,2 1,-1-1,0 1,0 0,1-1,-1 1,1 0,0 0,0 0,0-1,0 1,1 0,-1 1,1-1,0 0,-1 0,1 0,1 0,-1 0,0 0,1 0,0 0,-1 0,1 0,0 0,1 0,-1-1,0 1,1 0,0 0,0 1,-1-1,1 0,0-1,0 1,0 0,0 0,0-1,1 1,-1-1,1 0,0 0,-1 0,1 0,0 0,0 0,0-1,1 0,-1 1,0-1,0 0,1-1,-1 1,1-1,0 1,1-1,0-1,-1 0,1 0,0 0,0 0,-1-1,1 0,-1 0,1 0,-1 0,0-1,0 1,0-1,0 0,-1 0,4-4,5-4,0 2,1-1,0 2,0 0,0 0,1 1,1 1,-1 0,1 1,0 1,0 0,0 1,10 0,-3-1,-14 2,1 0,1 1,-1 0,0 0,0 1,0 0,4 1,-11 0,0-1,-1 1,1-1,0 1,0 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 1,0-1,1 0,-1 1,0-1,0 1,0-1,0 1,0 0,0-1,-1 1,1 0,0 0,-1 0,0-1,1 1,-1 0,0 0,0 0,0 0,0 0,0-1,0 1,-1 0,1 0,-1 0,0 1,1 1,-1 1,0-1,0 0,0 1,-1-1,1 0,-1 0,0 0,0 0,-1-1,1 1,-1 0,0-1,0 0,0 1,0-1,0-1,-1 1,-2 1,3-2,0 0,-1-1,1 0,0 0,-1 0,1 0,-1-1,1 1,-1-1,1 0,-1 0,1 0,-1-1,1 1,-1-1,1 0,-1 1,1-2,0 1,0 0,-1-1,1 1,0-1,0 0,0 0,-16-11,4 3,1 0,-1 1,0 0,-1 1,0 1,-1 1,1 0,-1 1,-5 0,21 5,0 0,-1 0,1 0,0-1,-1 1,1 0,0 0,0-1,-1 1,1-1,0 1,0-1,0 0,0 1,0-1,0 0,0 0,0 1,-1-2,2 2,0-1,0 0,0 1,0-1,0 1,0-1,0 0,0 1,0-1,1 1,-1-1,0 1,0-1,0 0,1 1,-1-1,0 1,0-1,1 1,-1-1,1 1,-1 0,0-1,1 1,-1-1,1 1,0 0,3-4,0 1,0 1,0-1,1 0,-1 1,1 0,-1 0,6-1,-1 1,0 0,0 1,0 0,1 0,-1 1,0 0,8 1,-15 0,1-1,0 1,-1-1,1 1,-1 0,1 0,-1 0,0 1,1-1,-1 0,0 1,0 0,0-1,0 1,0 0,0 0,0 0,-1 0,1 0,-1 1,0-1,1 0,-1 1,0-1,0 1,-1-1,1 1,0 2,1 10,-1 0,0-1,-1 1,-1 3,0 6</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1553.15">362 163,'0'5,"0"5,0 6,0 5,0 3,0 2,0 2,0-1,0 1,0-1,4-4,2-2,0-4</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink21.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:21:17.639"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#AB008B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'11'1,"1"1,-1-1,1 2,-1 0,0 0,0 1,0 0,0 1,-1 0,1 1,-1 0,-1 0,1 2,-7-7,11 7,0-2,1 1,0-2,0 0,4 0,45 16,-55-17,1-1,-1 0,1-1,0 0,4 0,7 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="794.68">28 26,'4'0,"2"5,4 1,1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink22.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:21:27.524"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#AB008B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">56 39,'-2'50,"0"-11,6-68,-4 27,1 0,-1 0,0 0,0 0,1 0,-1 0,1 1,0-1,-1 0,1 0,0 0,0 1,0-1,0 0,1 1,-1-1,0 0,0 2,0 0,0-1,-1 1,1 0,0-1,0 1,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,0 1,0-1,-1 0,1 1,0-1,0 1,-1-1,1 1,3 2,0 0,0 0,-1 0,1 1,-1-1,0 1,0 0,-1 0,1 0,-1 0,0 1,1 1,-1-2,-1-1,1 1,0-1,0 0,0 0,1 1,-1-1,1-1,0 1,0 0,0-1,0 1,0-1,1 0,-1 0,1 0,-1-1,1 1,0-1,-1 0,1 0,0 0,1 0,-14-2,2 1,1 0,-1 0,1-1,0 0,-1-1,-2-1,8 3,0 0,0-1,0 1,0 0,0-1,1 1,-1-1,0 0,0 1,1-1,-1 0,0 1,1-1,-1 0,0 0,1 0,-1 1,1-1,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 1,0-1,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 1,0-1,-1 0,1 1,0-1,0 0,27-31,-28 31,1 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 1,0-1,0 1,0-1,0 1,0-1,0 1,1 0,-1-1,0 1,0 0,1 0,-1 0,0 0,0 0,0 0,1 0,-1 1,0-1,0 0,0 1,1-1,-2 1,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1-1,-1 1,0 0,1 0,-2 0,-19 28,16-23,-14 18,28-43,-3 9,27-42,-32 51,-1 1,1-1,-1 0,1 1,-1-1,1 0,0 1,-1-1,1 1,0-1,-1 1,1-1,0 1,0-1,-1 1,1 0,0-1,0 1,0 0,0 0,-1 0,1-1,0 1,0 0,0 0,0 0,0 1,-1-1,1 0,0 0,0 0,0 1,0-1,-1 0,1 1,0-1,0 0,-1 1,1-1,0 1,-1 0,1-1,0 1,-1-1,1 1,-1 0,1-1,-1 1,1 0,-1 0,0 0,1-1,-1 1,0 0,0 0,1 0,-1 0,0 0,4 13,-1 0,-1 0,0 0,0 1,-2-1,0 0,0 1,-1-1,-1 0,-1 0,0 0,-4 14,7-28,0 1,-1 0,1 0,0 0,0 0,0-1,-1 1,1 0,-1 0,1 0,0-1,-1 1,1 0,-1-1,0 1,1 0,-1-1,1 1,-1-1,0 1,0-1,1 1,-1-1,0 0,0 1,1-1,-1 0,0 1,0-1,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,0 0,1 0,-1 0,0-1,0 1,0 0,0-1,1 1,-1 0,0-1,1 1,-1-1,0 1,0-1,1 0,-1 1,1-1,-1 0,1 1,-1-1,1 0,-1 1,1-1,-4-4,1 0,-1 0,1 0,0 0,0 0,1-1,0 1,-1-3,1-2,1 1,0 0,0-1,1 1,0-1,1 1,0-4,0 9,-1 0,1 0,0 0,0 0,0 0,1 1,-1-1,1 0,0 1,0-1,0 1,0 0,1 0,-1 0,1 0,0 0,0 0,1-1,-3 4,-1-1,1 1,0-1,-1 1,1-1,0 1,0 0,-1-1,1 1,0 0,0-1,-1 1,1 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,-1 0,1 1,0-1,0 0,0 0,-1 1,1-1,0 1,0-1,-1 1,1-1,-1 1,1-1,0 1,-1-1,1 1,-1 0,1-1,-1 1,1 0,-1 0,0-1,1 1,-1 0,0 0,0-1,0 1,1 0,-1 0,0 0,0 0,0-1,0 1,0 0,0 0,-1 0,2 6,-1-1,-1 0,1 1,-1-1,0 1,0-1,-1 1,-3 5,0-1,-1 1,0-1,-3 4,3-6,0 1,1 0,0 0,0 1,-2 9,7-18,0-1,-1 1,1 0,0 0,-1-1,0 1,1 0,-1-1,0 1,0-1,0 1,0-1,0 1,0-1,-1 1,1-2,1 0,-1-1,1 1,-1 0,1-1,-1 1,1 0,-1-1,1 1,0-1,-1 1,1-1,-1 1,1-1,0 1,0-1,-1 1,1-1,0 1,0-1,0 1,-1-1,1 0,0 1,0-1,0 1,0-1,-6-60,5 47,2-4,-2 0,0 1,-1-1,-2-5,2 16,0 0,-1 1,0-1,1 1,-2 0,1 0,-1 0,0 0,0 0,-1 1,0 0,-3-4,-13-6,21 15,-1 0,1 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 0,0 0,0 0,0 0,-1 0,1 0,0 1,0-1,0 0,0 0,0 0,0 0,-1 0,1 0,0 1,0-1,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,1 0,-1 0,0 1,0-1,0 0,0 0,0 0,23 47,-12-25,-1 1,27 68,-42-103,1 3,1 0,0 0,0 0,0-1,1 1,1-2,-1-6,-1-1,0 0,-1 1,-2-2,4 13,0 1,0 0,-1 0,0 0,0 0,0 0,0 0,-1 1,0 0,0 0,0 0,0 0,-1 1,1-1,-2 1,6 2,-1 1,0-1,1 1,-1 0,1-1,-1 1,0 0,1-1,-1 1,0 0,0 0,1 0,-1 0,0 0,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,0 0,1 1,-1-1,0 0,1 0,-1 1,0-1,0 1,-9 21,5 34,5-52,-1 31,3 87,-1-109,1-1,0 0,1 1,0-1,0 0,1 0,1-1,2 4,-7-14,0-1,1 1,-1 0,0-1,1 1,-1 0,0-1,1 1,-1 0,1-1,-1 1,1-1,0 1,-1-1,1 1,0-1,-1 1,1-1,0 0,-1 1,1-1,0 0,-1 0,1 1,0-1,0 0,0 0,-1 0,1 0,0 0,0 0,0-1,1 1,-1-1,1 0,-1 0,0 0,0 0,1 0,-1 0,0-1,0 1,0 0,0 0,0-1,0 0,23-53,-23 52,40-111,-41 113,0 1,0 0,0-1,0 1,1 0,-1-1,0 1,0 0,0-1,0 1,0 0,1-1,-1 1,0 0,0 0,0-1,1 1,-1 0,0-1,0 1,1 0,-1 0,0 0,1-1,-1 1,0 0,1 0,-1 0,0 0,1 0,-1 0,0 0,1-1,-1 1,0 0,1 0,-1 0,0 0,1 1,7 12,-1 22,-6-5,-1-1,-1 1,-2-1,-1 0,-1 0,-5 16,9-43,1-1,0 1,0 0,-1-1,1 1,0 0,-1-1,0 1,1-1,-1 1,0-1,0 1,0-1,0 0,0 1,-1 0,1-2,0-1,1 1,-1 0,1-1,-1 1,1-1,-1 1,1 0,-1-1,1 0,-1 1,1-1,0 1,-1-1,1 1,0-1,-1 0,1 1,0-1,0 0,0 1,0-1,-1 0,1 1,0-2,-8-59,7 45,3-89,-1 95,0 0,1 0,0 1,1-1,0 1,0 0,1-1,0 2,2-5,-3 10,0 1,0-1,0 0,0 1,0-1,0 1,1 0,-1 0,1 0,-1 1,1-1,0 1,0 0,-1 0,1 0,3 0,33-14,-44 14,-1-1,1 1,0 0,-1 0,1 0,-1 1,1-1,-1 1,1 0,-2-1,-1 1,1 0,0 0,0 0,0 1,-1-1,1 1,0 1,0-1,0 1,0 1,1-1,-1 1,0-1,1 2,0-1,0 1,0-1,0 1,-3 4,8-8,0 0,0 1,-1-1,1 0,0 0,0 1,-1-1,1 0,0 0,-1 0,1 1,0-1,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,-1-1,1 1,0 0,0 0,-1 0,1-1,0 1,0 0,-1 0,1-1,0 1,0 0,0-1,-1 1,1 0,0-1,-11-27,-1-37,10 41,0 2</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink23.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:22:40.753"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#AB008B"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">13 122,'9'-1,"-1"-1,1 0,0-1,-1 0,1 0,-1-1,0 0,0-1,-1 0,1 0,2-2,30-18,-11 3,6-5,-34 26,0 1,1-1,-1 1,0 0,1-1,-1 1,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,0 1,1-1,-1 1,0-1,1 1,-1-1,0 1,0 0,1 0,-1 0,0-1,0 2,0 0,0-1,0 1,0 0,0-1,-1 1,1 0,-1 0,0 0,1-1,-1 1,0 0,0 0,0 0,0 0,0-1,-1 1,1 0,0 0,-1 0,1-1,-1 1,0 0,0-1,0 1,0 0,0-1,-1 2,-31 47,31-48,-6 8,0-1,-1-1,0 1,-6 3,-32 32,44-40,0 0,0 0,0-1,0 1,-1-1,1 1,-1-1,0 0,0 0,0-1,-1 1,1-1,-1 0,1 0,-1 0,1-1,-4 1,7-2,1 0,0 0,0 0,-1 0,1 0,0 0,0 0,-1 0,1 0,0 0,0-1,0 1,-1 0,1 0,0 0,0 0,0 0,-1-1,1 1,0 0,0 0,0 0,0 0,-1-1,1 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0-1,0 1,0 0,0 0,0 0,8-21,14-16,19-24,-77 90,29-24,0 0,-1 0,2 0,-1 1,1 0,-1 1,2-1,-1 1,1 0,0 0,-1 4,5-11,1 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,0 0,0 1,0-1,0 0,1 0,-1 0,0 0,0 0,0 1,0-1,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 1,0-1,1 0,-1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,0 0,1 0,-1 0,0 0,0 0,16-4,13-9,4-7,1 1,0 2,2 1,32-9,-39 6,-26 17,-1 0,0 0,1 0,-1 1,1-1,0 1,0-1,-1 1,4-1,-7 5,0 0,0-1,-1 1,1-1,-1 1,1-1,-1 0,0 1,0-1,0 0,0 0,0 0,0 0,-3 1,-1 1,1 0,-1 1,1-1,-1 1,2 0,-1 1,-2 2,7-7,-1 1,0-1,1 1,-1-1,1 0,-1 1,1 0,0-1,-1 1,1-1,0 1,0-1,0 1,0-1,0 1,1 0,-1-1,0 1,1-1,-1 1,1-1,0 0,-1 1,1-1,0 1,0-1,0 0,0 0,0 0,0 1,0-1,0 0,1 0,-1 0,0-1,0 1,1 0,17 12,-15-10,1-1,-1 1,0 1,0-1,0 0,-1 1,1 0,0 1,-10-9,0 0,0 1,0 0,-1 0,1 1,-1-1,1 1,-1 1,0-1,0 1,-49-16,45 11,-27-10,38 16,-1 0,1 0,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,-1 0,1 0,-1 1,1-1,-1 0,1 0,-1 1,1-1,-1 0,1 0,-1 1,1-1,0 1,-1-1,1 0,-1 1,0 22,4-17,0 0,0 0,0 0,1 0,0-1,0 1,1-1,0 0,-1 0,2-1,-1 0,0 1,1-2,0 1,0-1,0 0,6 2,-12-5,1 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,0-1,-1 1,1 0,-1-1,1 1,-1 0,1-1,-1 1,1 0,-1-1,1 1,-1-1,0 1,1-1,-1 1,0-1,1 1,-1-1,0 1,0-1,1 0,-1 1,0-1,0 1,0-1,0 0,0 1,0-1,0 1,0-1,0 0,2-29,-2 26,0-23,-1 14,1 1,0-1,1 1,0-1,1 1,0-1,1 1,1 0,0 0,2-3,-5 14,0-1,-1 1,1 0,0-1,0 1,-1-1,1 0,-1 1,0-1,1 1,-1-1,0 0,0 1,0-1,0 0,0 1,0-1,0 0,-1 1,1-1,-1 1,1-1,-1 1,0-1,1 1,-1-1,-1 1,1-1,-1 1,0 0,1 1,-1-1,0 0,0 0,0 1,0-1,1 1,-1-1,0 1,0 0,0 0,0 0,0 0,0 0,0 0,0 1,0-1,0 1,1-1,-2 1,-3 1,0 0,1 0,-1 1,0 0,1 0,-1 0,1 0,0 1,0 0,1 0,-5 5,-2 4</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink24.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:25:42.783"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#33CCFF"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink25.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T09:25:50.274"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#33CCFF"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">106 264,'55'-21,"-30"13,1 1,0 1,0 2,0 0,1 1,-1 2,2 1,18 1,-1-3,0-1,32-7,-21 3,0 2,0 2,51 6,-12-2,-72 1,0 0,-1 2,19 5,9 1,187 43,-111-23,-38-8,37 9,-78-17,1-3,0-1,0-3,31 0,-57-5,-1 1,0 1,0 1,-1 0,13 6,42 11,-37-12,-1 2,4 3,-18-6,1 0,1-2,-1-1,1 0,0-2,2-1,-5-2,-1 1,0 1,1 1,-2 1,1 1,0 0,6 4,-19-5,17 8,0-1,1-1,1-1,-1-2,7 1,99 18,-82-16,1 1,16 8,57 15,-81-24,-25-6,-1-1,1-1,-1 0,2-1,5 1,-1 1,1 1,-1 1,0 1,9 5,56 15,-34-13,-1 2,0 2,19 11,0 1,27 5,37 14,-81-28,47 10,-79-25,81 28,-62-19,0-2,1-2,12 1,-39-8,0 0,-1 2,0 0,0 1,0 0,-1 1,13 10,35 18,4-4,174 80,-184-89,43 17,93 53,-103-46,-55-31,-1 1,-1 2,0 1,-2 1,18 17,84 68,-116-92,1 0,1-1,0-1,8 4,-5-4,-2 1,1 1,10 10,2 3,1-1,1-3,12 6,-14-9,-1 1,0 1,-2 2,8 9,100 94,-56-49,51 45,-25-7,30 9,-103-95,15 17,-14-1,20 39,-33-49,1-1,2-1,2-1,7 6,-27-32,-1 1,0 0,-1 1,1 0,1 5,18 27,17 10,-27-34,-1 1,0 0,5 12,6 14,2-1,2-1,1-1,11 8,-28-33,0 1,-2 0,0 0,0 1,-2 1,0 0,0 3,18 38,4-8,-22-38,-1 0,0 0,0 1,3 12,12 33,4 0,23 39,3 6,-21-48,-24-44,0-1,-1 2,-1-1,0 1,-1 0,0 0,2 14,-4-13,2 0,-1 0,2 0,6 12,14 42,45 204,-60-228,-2 1,-2 0,-1 1,-3-1,-2 5,-2 1088,0-1119,-2 0,1 0,-6 15,4-14,0 1,1 0,1 2,1 14,1-7,-1-1,-2 0,-1 0,-3 8,-17 81,15-67,-2 0,-18 48,-50 86,66-156,-5 9,-1-2,-11 16,-119 195,127-210,15-25,-1 1,-1-2,0 1,-8 8,5-7,1 1,0 0,1 1,-4 8,6-8,-1-1,-1 0,-1 0,0-1,-1 0,-24 24,-33 31,49-51,1 2,1 0,1 1,0 2,-52 59,-16-12,56-48,2 0,-5 8,0-2,-1 0,-35 21,-51 20,20-12,54-31,-1-2,-12 3,-57 29,43-20,-43 14,49-22,40-18,0-2,-25 6,-33 9,37-9,-1-1,-30 2,-7 2,-74 10,27-1,-53 0,155-21,1-2,-1 0,-11-2,13 0,-1 0,1 2,-22 6,19-4,-1-1,1-1,0-1,-17-3,16 0,1 2,-1 1,0 2,-13 3,-113 21,115-22,0-1,0-2,-1-1,0-3,-1-2,-54 0,69 5,-1 1,-27 6,27-4,-1 0,-23-2,29-2,-22-2,1 3,-1 2,-22 6,35-5,0-2,-1-1,-30-3,-52 3,46 11,52-9,0 0,0-1,-7-1,-39-1,33-2,1 2,0 1,1 1,-24 7,28-5,-1-1,1-1,-25-2,23 0,0 1,0 1,-14 4,-142 20,139-19,-1-3,1-2,-1-2,1-2,-2-2,-59 0,-608 3,695 2,0 0,0 1,-14 4,12-3,0 0,0-1,-2-1,-374-3,378 0,0-1,0-1,-15-4,14 2,-1 2,0 0,-2 1,-214 2,215 0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1487.38">900 8943,'-51'0,"11"-1,0 1,0 3,1 1,-28 6,-16 13,-23 12,-47 14,114-39,15-4,0 0,0 2,0 1,1 0,-16 11,15-10,21-10,0 1,0 0,1 0,-1 0,0 0,0 1,1-1,-1 1,1 0,-1 0,1-1,0 2,-1-1,1 0,2-1,0 0,0 0,0-1,0 1,0 0,0 0,0 0,0 0,1-1,-1 1,0 0,0 0,1 0,-1-1,0 1,1 0,-1-1,1 1,-1 0,1-1,-1 1,1 0,0-1,-1 1,1-1,0 1,-1-1,1 1,0-1,0 0,-1 1,1-1,31 16,-24-12,54 28,23 7,53 8,-77-28,-15-3,-29-9,0-1,1-1,0 0,0-1,0-1,0-1,1-1,14 2,-1 0,19 6,18 3,86 13,-156-24</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="29494.74">292 264</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="30796.04">1 238,'3'0,"0"-1,0 0,0-1,0 1,-1 0,1-1,0 0,0 0,-1 0,1 0,-1 0,2-2,21-14,-5 9,1-2,-2 0,1-2,4-4,-9 7,89-44,2 1,-89 45,-1 1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="31903.9">1 264,'0'2,"1"-1,-1 1,1-1,-1 0,1 1,0-1,0 0,-1 0,1 0,0 0,0 0,0 1,0-2,1 1,-1 0,0 0,0 0,1 0,-1-1,32 17,-25-13,115 63,-87-48,-29-14,1-1,0 0,0-1,0 1,0-2,1 1,-1-1,3 0,30 5,-1 2,3 3,48 9,-72-17</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="33542.01">503 0,'0'5,"0"5,0 6,0 5,0 3,0 2,0 1,0 1,0-1,0 1,0-1,0 0,0 0,0-1,0 1,0-1,0-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="34594.26">900 8757,'0'5,"4"1,2 4,0 6,-1 3,-2-1</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="34903.33">953 8969,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="35897.55">953 8995,'0'5,"0"6,0 5,0 5,0 3,0 2,0 1,0 1,0-1,0 1,0-1,0 0,0-1,0-4</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="37387.02">927 9234,'4'0,"2"5,4 1,1 4,-2 5,-3 4,-1 4,2-2,0-1,-1-3</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink3.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T08:26:03.749"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#F6630D"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 298,'0'-2,"0"0,1 0,0 0,-1 1,1-1,0 0,0 0,0 0,0 0,0 1,0-1,1 1,-1-1,1 1,-1-1,1 1,1-1,37-26,-18 14,6-5,2 2,0 0,1 3,0 0,1 2,1 1,9-1,58-21,-77 26,1 1,-1 1,7 0,23-5,133-16,-140 19,1 2,0 2,-1 2,48 5,13-2,-5-3,-24-1,59 6,-66 9,-52-8,0-2,1 0,10 0,-2-1,0 2,23 6,1 0,-1 1,0 2,47 19,29 8,-77-25,0 2,-1 2,45 25,-17-12,-59-26,0 1,-1 1,0 0,0 1,-1 1,6 5,-2-1,1-1,1 0,0-2,15 6,59 32,30 23,4-6,116 41,-6-3,69 18,-52-23,-203-79,1-1,12-1,-24-7,-1 2,-1 1,0 2,18 12,67 28,-116-48,-1 0,0 1,-1 0,0 1,0-1,-1 1,0 1,-1 0,0-1,2 9,16 23,0 3,-2 0,16 45,-17-37,2-1,7 7,-9-19,-2 1,-1 2,-3-1,9 39,7 41,1 37,-21-104,3 24,0 8,-9-63,-1 0,0 25,-4 37,-1-48,1 0,2-1,2 1,6 27,-4-31,-2-1,-1 1,-2 0,-2-1,-1 11,0 4,2 0,2 3,25 83,-17-76,-4-26,-1 1,0 28,-2-25,1-1,3 10,-1-11,-2 0,0 21,-2-15,2 0,3 8,-2-9,0 0,-2 18,-4 580,-1-617,0 0,0 0,-6 14,4-12,0 0,1 0,1 2,1 29,2-22,-2 0,-2 0,-1 0,-4 15,-19 139,1 0,-1-27,21-119,2 1,1-1,2 1,2-1,2 5,-1 11,-1 1,-4 5,-10 11,9-53,0 1,1 1,1 6,1 2,-1 0,-1 0,-7 27,-17 102,15-82,10-55,-1-1,-1 1,-1-1,0 0,-3 2,1 0,1 1,0 0,2 0,1 0,-1 17,-6 46,-52 231,52-271,4-18,1-1,1 1,0 28,2-18,-2 0,-6 26,-1 8,0-2,6-43,0 0,2 0,2 7,-1-6,0-1,-2 1,0-1,-2 0,-1-1,-2 1,0-1,-9 15,-11 35,22-60</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1703.38">4472 7680,'3'0,"1"1,-1-1,1 1,-1-1,0 1,1 0,-1 0,0 1,1-1,-1 0,0 1,0 0,0 0,0 0,-1 0,1 0,-1 1,1-1,0 1,5 8,-1-1,0 1,0 0,3 9,17 27,-16-30,-1 2,-1 0,-1 0,-1 1,0 0,-1 0,-1 0,-1 4,23 74,3-19,-10-29,-2 0,9 47,-26-93,20 74,-19-74,0 1,0-1,0 0,0 0,1 0,-1 0,1 0,0 0,1-1,-1 1,0-1,1 0,0 0,0 0,0 0,-3-3,0 0,0 1,0-1,1 0,-1 0,0 0,0 1,0-1,0 0,1-1,-1 1,0 0,0 0,0 0,0-1,0 1,0 0,0-1,0 1,1-1,-2 0,1 1,0-1,0 0,0 0,0 1,0-1,0 0,-1 0,1 0,0 0,-1 0,1 0,-1 0,1 0,-1-1,23-49,-16 32,0 2,-1-1,-1 0,-1 0,0 0,0-5,-1 2,1 0,1 0,7-18,27-66,-20 51,2 0,3 2,3-3,-21 42,0 0,-1-1,-1 1,0-1,-1 0,0-3,-2 5,1 1,1 0,0 0,0 1,1-1,0 0,1 1,0 0,1 0,1-1,4-1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink4.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T08:26:43.580"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#F6630D"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 403,'0'-1,"0"-1,0 0,1 0,-1 1,1-1,0 0,-1 1,1-1,0 1,0-1,0 1,0-1,0 1,0-1,1 1,-1 0,0 0,1 0,-1 0,1 0,-1 0,1 0,43-20,-20 11,21-16,0 3,2 2,1 2,24-5,39-4,57-6,-58 9,-80 17,0 1,1 1,0 2,22 0,-32 3,0-1,-1-2,9-1,61-8,32-1,-83 8,-1 2,23 0,-37 4,1-1,-1-1,0-1,18-5,-14 3,0 1,1 1,27 2,-27 1,-1-2,1 0,27-7,-11 1,0 3,1 2,-1 2,1 2,1 2,58-1,1056-2,-1122 2,0 2,16 4,-16-2,1-2,10-1,92-5,-51-1,68 8,-89 8,-51-9,0 0,0-1,8-1,91-3,-59-1,52 5,-42 10,-51-8,0-2,1 0,12 0,116-2,-55-2,1 4,37 9,39 8,0-7,77-8,-159-5,1 5,17 5,25 1,1-6,69-8,-21 0,-89 7,26 6,-30-1,46-4,-11-8,-12 0,80 9,-119 7,-51-9,0 0,0-1,7-1,22-1,-1 2,41 9,-38-5,51 2,21 2,148 15,112 12,-284-27,13 6,55 7,217 30,-205-27,-12-1,-87-15,-35-5,1-1,21-2,-41-1,-1 0,1 2,6 2,-3-1,-1-1,16 0,-14-3,0 1,0 1,25 6,-26-3,0-2,17 0,-16-2,-1 1,18 5,172 30,-14-3,52 17,-140-29,20-2,50 9,390 82,72 11,302 50,-817-150,17-3,-67-10,40 12,-81-14,0-2,20-1,61 9,19 12,-118-21,0-2,0-1,0-1,4-1,-3 0,1 1,-1 1,20 4,199 35,-21-4,64 7,-42-8,127 17,247 53,-375-70,33 7,-89-8,158 33,-193-38,3-7,-82-12,-64-10,137 22,80 24,47 14,46 13,-76-9,201 63,-184-53,-51-17,382 128,-189-84,-364-92,204 51,164 36,-199-45,-188-47,1 0,-1 2,0 1,-1 1,1 0,-2 1,0 2,5 3,82 48,107 46,-96-52,74 52,137 88,-327-196,58 33,-10-7,29 23,122 77,-34-27,98 58,-59-46,-155-81,-2 2,18 17,-50-37,-2 1,1 0,-2 1,0 1,0 0,-2 1,0 0,7 15,87 154,-88-154,2-1,11 14,29 50,-11-16,-34-58,-1 1,-1-1,-1 2,-1 0,0 3,-2-7,0 0,1 0,2 2,21 45,-18-29,4 7,-3 1,6 27,2 8,-16-60,-1 0,0 1,-2 0,0 0,-1 6,0-4,0 1,2-1,1 0,4 11,-3-13,-1 1,-2 0,0 0,0 0,-2 5,0 4,2-1,1 0,1-1,3 6,-1-7,-2 1,0 1,-3-1,1 18,-4 2,-2-15,3 1,1 0,1-1,7 29,-2-18,-3 0,-2 1,-2 0,-1 0,-3 5,0 56,3 423,1-511,1 0,1 1,4 16,-2-15,-1 0,-1 1,-1 4,-2 106,0-109</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1350.3">25480 7203,'1'5,"0"0,1 0,-1-1,1 1,0-1,1 0,-1 1,1-1,1 2,9 16,29 51,-31-56,0 0,-2 1,0 0,5 13,-7-12,2 0,1 0,0-1,1-1,9 11,-6-8,-1 0,0 0,5 16,-18-35,1-1,-1 1,0-1,0 1,0-1,0 1,0-1,1 0,-1 1,0-1,0 1,1-1,-1 0,0 1,1-1,-1 0,0 1,1-1,-1 0,0 0,1 1,-1-1,1 0,-1 0,1 0,-1 1,1-1,-1 0,0 0,1 0,0 0,9-12,9-37,-12 27,124-222,-123 229</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink5.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T08:29:38.781"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#F6630D"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1188 159,'19'0,"17"0,0 0,0 3,0 1,23 6,285 70,-185-54,97 36,-196-49,0 2,46 19,60 41,-128-57,-1 2,-1 1,5 6,-13-6,-1 1,-2 2,0 1,-1 1,-1 0,-2 2,11 18,-11-16,-1-1,1 0,2-1,7 6,50 71,-57-76,-1 1,-1 1,-2 1,14 30,20 33,27 64,-27-54,-1 1,-34-71,-3 1,-1 1,4 16,-5-12,2-1,14 25,9 29,-9-21,-23-55,-1-1,0 1,-1 1,1 12,4 16,18 47,-16-58,-1 2,-1 1,-7-27,10 51,-3 1,-3 0,-2 19,-4-58,0-1,3 1,0-1,5 22,0-1,-3 2,-2-1,-2 0,-1 1,-4 2,2 57,3-4,1-21,-6 53,-22-2,19-98,-2-1,-1 0,-6 11,-9 26,11-21,6-19,-2-1,-6 12,-20 48,21-48,-3 0,-16 28,-39 70,43-80,24-45,-1 0,0 0,-1-1,-7 9,-7 8,2 1,-6 15,8-16,0 0,-21 24,-34 45,48-62,-2-1,-23 23,-55 74,81-106,1 2,2 1,1 1,-7 17,13-25,-20 28,-2-3,-2-1,-2-1,-28 23,32-28,28-31,0-1,-1 0,1 0,-2 0,1-1,-1-1,0 0,-2 1,-2 0,1 1,0 0,0 1,-8 9,-24 19,-18-5,21-12,-7 8,28-16,-2 0,1-1,-17 5,14-6,1 1,0 1,-10 7,14-6,-2-2,1-1,-2 0,-11 2,9-2,-1 0,2 2,0 0,-7 7,-41 21,5 0,-19 8,-22 4,93-46</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="296.06">1426 6430,'-5'0,"-1"5,-4 1,-5-1,-5 0,2-2</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1496.42">1479 6112,'-1'10,"0"0,0-1,-1 1,0-1,-1 0,0 0,0 0,-1 0,0 0,-1-1,0 1,-2 2,-10 11,0 0,-1-1,-16 13,14-11,1 1,1 0,1 1,-4 11,-16 22,-28 29,65-86,-1-1,1 1,0-1,-1 1,1-1,-1 1,1 0,0-1,-1 1,1-1,0 1,0 0,-1-1,1 1,0 0,0 0,0-1,0 1,0 0,0-1,0 1,0 0,0-1,0 1,1 0,-1-1,0 1,0 0,1-1,-1 1,0 0,1-1,-1 1,0-1,1 1,1 0,0 0,-1-1,1 1,0 0,0-1,0 0,0 0,0 1,-1-1,1 0,0 0,0-1,1 1,56-13,11-11,-35 11,1 2,11-1,162-41,-40 9,-151 39</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="3656.92">1637 0,'-1637'0,"1646"2,0 0,-1 0,0 0,1 1,-1 0,0 1,0 0,25 9,46 18,-54-20,0-1,1-1,9 2,12 2,-2 1,1 3,0 3,85 31,81 15,-17-6,-153-45,394 117,-411-128,0 0,0-2,0-1,0 0,12-3,1 1,-15 1</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink6.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T08:36:25.258"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#66CC00"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink7.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T08:36:25.881"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#66CC00"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink8.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T08:36:26.286"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#66CC00"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 0,'0'0</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="295.06">1 26,'0'0</inkml:trace>
+</inkml:ink>
+</file>
+
+<file path=xl/ink/ink9.xml><?xml version="1.0" encoding="utf-8"?>
+<inkml:ink xmlns:inkml="http://www.w3.org/2003/InkML">
+  <inkml:definitions>
+    <inkml:context xml:id="ctx0">
+      <inkml:inkSource xml:id="inkSrc0">
+        <inkml:traceFormat>
+          <inkml:channel name="X" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+          <inkml:channel name="Y" type="integer" min="-2.14748E9" max="2.14748E9" units="cm"/>
+        </inkml:traceFormat>
+        <inkml:channelProperties>
+          <inkml:channelProperty channel="X" name="resolution" value="1000" units="1/cm"/>
+          <inkml:channelProperty channel="Y" name="resolution" value="1000" units="1/cm"/>
+        </inkml:channelProperties>
+      </inkml:inkSource>
+      <inkml:timestamp xml:id="ts0" timeString="2020-06-01T08:57:19.696"/>
+    </inkml:context>
+    <inkml:brush xml:id="br0">
+      <inkml:brushProperty name="width" value="0.05" units="cm"/>
+      <inkml:brushProperty name="height" value="0.05" units="cm"/>
+      <inkml:brushProperty name="color" value="#66CC00"/>
+      <inkml:brushProperty name="ignorePressure" value="1"/>
+    </inkml:brush>
+  </inkml:definitions>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0">1 5774,'1589'0,"-1570"2,1 0,-1 0,18 6,-17-3,1-1,1-1,4-1,5-1,-1 1,1 1,20 6,-21-3,0-2,16 0,-15-2,0 1,13 5,-14-4,0 0,1-2,-1-1,16-2,-15 0,0 1,-1 2,0 0,15 5,172 30,-11-15,-172-17,1-2,0-1,18-3,54 3,26 23,-47-11,-63-9,1-1,-1-1,6-1,95 11,-83-7,0-1,17-3,28-3,-24-1,55 5,-46 10,-52-8,0-2,1 0,10 0,652-1,-332-5,735 3,-1065 2,0 0,0 1,15 4,-14-3,1 0,0-1,2-1,54-2,-44-1,0 2,-1 1,1 1,29 8,-22-4,1-2,0-2,-1-1,1-3,13-2,42 0,-96 3,34 0,0 1,0 1,0 2,20 5,-10-2,1-1,-1-3,1-2,0-2,5-2,56 0,766 3,-852-1,-1-1,0-1,14-4,-12 2,0 2,0 0,2 1,5 1,0-1,-1-1,29-7,-12 3,1 1,0 3,0 2,0 1,5 4,56-2,-23 0,-16-1,43-4,-39-10,-52 9,0 0,0 1,7 1,-9 1,12 1,0-2,0-1,0-1,2-2,-6 1,0 2,0 1,0 0,4 2,-3 0,0-1,0-1,12-4,126-32,-101 25,29-13,-61 17,6-1,-14 4,-1 0,0-2,6-4,40-12,-60 22,0 0,0-1,0 0,-1 0,1-1,-1 0,0 0,0-1,0 0,-1-1,1 0,-1 0,-1 0,1-1,1-3,9-16,-2 0,0-1,2-11,30-53,-38 73,-1-1,-1 0,0-1,-2 0,0 0,-1-1,8-31,19-43,7-24,-28 78,-5 24,-1-1,-1 1,0-1,-1-2,23-139,-11 72,-9 64,-1 0,-1 0,-1-5,-1-24,-1 20,1 0,1 0,2 0,3-11,-2 14,-1 0,-1 0,-2-29,-1 28,2 0,1 1,5-28,-2 28,-2 0,0-18,-2 17,1 1,5-18,19-44,-15 54,-1-1,-2-2,8-37,8-17,-19 74,8-41,-10 40,1 1,0 0,2 0,2-5,1 1,-2-1,0 0,-2-3,18-53,-13 42,-1-1,-2 0,-1 0,0-39,-6 70,5-31,2 0,2 0,2 0,3-3,7-25,-20 62,9-29,-2 0,1-15,-1 4,2 2,12-30,2-11,34-175,-33 189,-17 52,-1-1,-2 0,1-4,5-18,2 0,2 1,1 1,10-15,3-6,-2-9,-19 43,2 1,11-20,12-17,-15 27,1 1,2 0,11-12,-21 30,-1 0,0-1,1-3,-5 5,2 1,0 1,1-1,1 2,0-2,17-17,-2-1,8-16,-12 17,1 2,1 0,5-2,55-65,-53 59,27-26,119-125,-35 53,-25 26,-106 100,1 0,0 1,0 1,1 0,11-5,20-12,1-16,-39 34,1 0,0 1,0 0,1 0,-1 0,5-2,2 2,1-1,-1 2,1 0,0 1,0 0,1 1,-1 1,10 0,29 0,48 5,-13-1,-50-2,-3-1,0 2,-1 1,1 2,30 7,-39-6,1-1,-1-1,13-1,-11-1,0 1,0 2,0 1,103 23,53-2,-53 0,-104-21,0-1,0-2,19 0,-19-2,0 2,-1 0,25 7,-22-4,0-1,0-1,0-2,9-1,-8 0,-1 1,1 1,-1 2,6 2,-4-1,0-1,0-1,0-2,1-2,3-1,10 1,44 3,-18 11,-53-8,0-2,0 0,11 0,371-2,-193-3,-187 4,-1 0,0 1,14 4,-12-3,0 0,0-1,2-1,534-1,-269-3,-269 4,-1 0,0 0,18 6,-16-3,0-1,0-1,6-1,567 0,-288-5,-287 2,1-1,-1-1,18-4,-16 2,0 1,0 1,5 1,-22 2,46-2,0-1,32-7,19-2,-67 10,-1-2,21-5,-24 3,1 2,-1 2,0 0,8 3,-7-1,-1-1,1-1,-1-2,7-2,9-2,0 3,0 2,1 2,-1 2,3 2,57-1,1006-2,-1092 2,0 0,0 1,15 4,-14-3,1 0,0-1,2-1,-1 0,0 1,0 1,0 0,-1 1,1-1,1-1,0-1,7-1,-1 1,0 1,23 6,-24-3,1-3,1 0,22-2,-24-1,0 1,0 2,0 1,3 2,-1-1,1-1,-1-1,1-2,0-1,9-2,5 0,42 4,-17 11,-51-9,0 0,0-1,7-1,51-2,-44-1,0 2,-1 1,1 1,29 8,-22-4,1-2,0-2,0-1,-1-3,14-2,42 0,1782 3,-1860-1,1-1,-1-1,18-4,-17 2,2 1,-1 1,5 1,656 0,-331 4,204-2,-547 1,0-1,0 1,0 0,0 0,0 1,0 0,-1 1,1 0,-1 0,0 0,0 1,0 0,0 0,-1 1,0 0,1 0,-2 1,1-1,-1 1,0 0,0 1,0-1,-1 1,0 0,-1 0,1 1,-1-1,-1 0,1 1,-1 0,-1 0,0 0,0-1,0 1,-1 5,13 105,-6-74,-3 1,-1 13,-4 498,1-533</inkml:trace>
+  <inkml:trace contextRef="#ctx0" brushRef="#br0" timeOffset="1118.25">26301 959,'-1'57,"3"73,0-114,0 0,1-1,1 1,0-1,1 1,1-1,1 1,44 111,-19-37,-26-70,0 0,2 0,0 0,1-1,5 6,-14-24,1 0,0 0,-1 0,1 0,0 0,-1 0,1 0,0 0,0-1,0 1,0 0,0-1,0 1,0-1,0 1,0-1,0 1,0-1,0 0,0 1,1-1,-1 0,0 0,0 0,0 0,1 0,0 0,0-1,0 0,0 0,1 0,-1 0,0 0,0 0,0 0,-1-1,1 1,0-1,0 1,0-1,8-10,0 0,-1 0,0-1,0-4,-2 6,18-26,-13 21,-1 0,-1-1,0-1,-1 0,5-16,-11 26,1 0,0 0,1 1,-1 0,1 0,1 0,2-3,23-32,-24 29,-1-1,0 0,-1 0,0 0,-1-1,-1 0,0 1,-1-3,22-116,-3 49,-17 64</inkml:trace>
+</inkml:ink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -961,19 +3382,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C6:N90"/>
+  <dimension ref="B7:N88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J67" workbookViewId="0">
-      <selection activeCell="M87" sqref="M87"/>
+    <sheetView tabSelected="1" topLeftCell="C40" workbookViewId="0">
+      <selection activeCell="I88" sqref="I88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="2" max="2" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="37.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="36.5703125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="24.140625" customWidth="1"/>
@@ -982,65 +3404,10 @@
     <col min="14" max="14" width="36" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="6" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C6" t="s">
-        <v>14</v>
-      </c>
-      <c r="D6">
-        <v>67586991</v>
-      </c>
-      <c r="E6" t="s">
-        <v>135</v>
-      </c>
-      <c r="F6" t="s">
-        <v>136</v>
-      </c>
-      <c r="G6" t="s">
-        <v>137</v>
-      </c>
-      <c r="H6" t="s">
-        <v>138</v>
-      </c>
-      <c r="I6" t="s">
-        <v>139</v>
-      </c>
-      <c r="J6" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="7" spans="3:12" x14ac:dyDescent="0.25">
-      <c r="C7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" t="s">
-        <v>15</v>
-      </c>
-      <c r="E7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F7" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" t="s">
-        <v>17</v>
-      </c>
-      <c r="H7" t="s">
-        <v>18</v>
-      </c>
-      <c r="I7" t="s">
-        <v>10</v>
-      </c>
-      <c r="J7" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" t="s">
-        <v>19</v>
-      </c>
-      <c r="L7" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="1"/>
+    </row>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C10" s="6" t="s">
         <v>14</v>
       </c>
@@ -1048,15 +3415,15 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C11" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="17">
         <v>67586991</v>
       </c>
     </row>
-    <row r="12" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C12" s="6" t="s">
         <v>16</v>
       </c>
@@ -1064,7 +3431,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="13" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C13" s="6" t="s">
         <v>2</v>
       </c>
@@ -1072,7 +3439,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="14" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C14" s="6" t="s">
         <v>17</v>
       </c>
@@ -1080,7 +3447,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="15" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C15" s="6" t="s">
         <v>18</v>
       </c>
@@ -1088,7 +3455,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:4" x14ac:dyDescent="0.25">
       <c r="C16" s="6" t="s">
         <v>10</v>
       </c>
@@ -1096,42 +3463,28 @@
         <v>139</v>
       </c>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C17" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="D17" t="s">
+      <c r="D17" s="32" t="s">
         <v>140</v>
       </c>
-    </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.25">
+      <c r="E17" s="12" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C18" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C19" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="3:7" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
-        <v>20</v>
-      </c>
-      <c r="D27" t="s">
-        <v>141</v>
-      </c>
-      <c r="E27" t="s">
-        <v>142</v>
-      </c>
-      <c r="F27" t="s">
-        <v>143</v>
-      </c>
-      <c r="G27" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="29" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C29" s="6" t="s">
         <v>20</v>
       </c>
@@ -1139,15 +3492,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C30" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D30" t="s">
+      <c r="D30" s="18" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="31" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C31" s="6" t="s">
         <v>10</v>
       </c>
@@ -1155,7 +3508,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="3:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="3:5" x14ac:dyDescent="0.25">
       <c r="C32" s="6" t="s">
         <v>2</v>
       </c>
@@ -1163,33 +3516,38 @@
         <v>143</v>
       </c>
     </row>
-    <row r="33" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C33" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="D33" t="s">
+      <c r="D33" s="17" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="34" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C34" s="6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="35" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C35" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C36" s="6" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C39" s="2"/>
     </row>
-    <row r="41" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C41" s="5" t="s">
         <v>35</v>
       </c>
@@ -1206,24 +3564,27 @@
         <v>52</v>
       </c>
     </row>
-    <row r="42" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="B42" s="12" t="s">
+        <v>157</v>
+      </c>
       <c r="C42" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D42" s="3" t="s">
+      <c r="D42" s="30" t="s">
         <v>145</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="E42" s="31" t="s">
         <v>149</v>
       </c>
       <c r="H42" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="I42" s="8" t="s">
+      <c r="I42" s="22" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="43" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C43" s="5" t="s">
         <v>2</v>
       </c>
@@ -1240,7 +3601,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="44" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C44" s="5" t="s">
         <v>37</v>
       </c>
@@ -1253,28 +3614,31 @@
       <c r="H44" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="I44" s="8" t="s">
+      <c r="I44" s="21" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="45" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C45" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="D45" s="3" t="s">
+      <c r="D45" s="19" t="s">
         <v>147</v>
       </c>
-      <c r="E45" s="4" t="s">
+      <c r="E45" s="20" t="s">
         <v>147</v>
       </c>
       <c r="H45" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="I45" s="10" t="s">
+      <c r="I45" s="22" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="46" spans="3:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="J45" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="46" spans="2:10" ht="45" x14ac:dyDescent="0.25">
       <c r="C46" s="5" t="s">
         <v>39</v>
       </c>
@@ -1291,11 +3655,11 @@
         <v>56</v>
       </c>
     </row>
-    <row r="47" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C47" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="D47" s="4" t="s">
+      <c r="D47" s="29" t="s">
         <v>148</v>
       </c>
       <c r="E47" s="3"/>
@@ -1303,7 +3667,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="49" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:10" x14ac:dyDescent="0.25">
       <c r="D49" s="12" t="s">
         <v>157</v>
       </c>
@@ -1311,7 +3675,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="51" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:10" x14ac:dyDescent="0.25">
       <c r="H51" s="10" t="s">
         <v>52</v>
       </c>
@@ -1319,15 +3683,15 @@
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:10" x14ac:dyDescent="0.25">
       <c r="H52" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="I52" s="14" t="s">
+      <c r="I52" s="33" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="53" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:10" x14ac:dyDescent="0.25">
       <c r="H53" s="10" t="s">
         <v>2</v>
       </c>
@@ -1335,7 +3699,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="54" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:10" x14ac:dyDescent="0.25">
       <c r="H54" s="10" t="s">
         <v>54</v>
       </c>
@@ -1343,302 +3707,266 @@
         <v>159</v>
       </c>
     </row>
-    <row r="55" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:10" x14ac:dyDescent="0.25">
       <c r="H55" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="I55" s="10" t="s">
+      <c r="I55" s="22" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="56" spans="4:14" x14ac:dyDescent="0.25">
+      <c r="J55" s="12" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="56" spans="4:10" x14ac:dyDescent="0.25">
       <c r="H56" s="10" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="57" spans="4:14" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:10" x14ac:dyDescent="0.25">
       <c r="H57" s="10" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="61" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="I61" s="6">
+    <row r="60" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="H60" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I60" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="H61" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I61" s="24" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="62" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="H62" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I62" s="8" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="63" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="H63" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I63" s="8" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="64" spans="4:10" x14ac:dyDescent="0.25">
+      <c r="H64" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="I64" s="35" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="65" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="H65" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="H66" s="6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="67" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="H67" s="6" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="70" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="I70" s="6">
         <v>1</v>
       </c>
-      <c r="J61" s="6">
-        <v>2</v>
-      </c>
-      <c r="K61" s="6"/>
-      <c r="L61" s="6"/>
-      <c r="M61" s="6">
-        <v>2</v>
-      </c>
-      <c r="N61" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="62" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H62" s="5" t="s">
+      <c r="J70" s="6">
+        <v>2</v>
+      </c>
+      <c r="K70" s="25"/>
+      <c r="L70" s="25"/>
+      <c r="M70" s="25"/>
+      <c r="N70" s="25"/>
+    </row>
+    <row r="71" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="H71" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I62" s="13" t="s">
+      <c r="I71" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="J62" s="13" t="s">
+      <c r="J71" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="L62" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="M62" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="N62" s="15" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="63" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H63" s="5" t="s">
+      <c r="L71" s="26"/>
+      <c r="M71" s="27"/>
+      <c r="N71" s="27"/>
+    </row>
+    <row r="72" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="G72" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="H72" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I63" s="13" t="s">
+      <c r="I72" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="J63" s="13" t="s">
+      <c r="J72" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="L63" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="M63" s="13" t="s">
-        <v>158</v>
-      </c>
-      <c r="N63" s="15" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="64" spans="4:14" x14ac:dyDescent="0.25">
-      <c r="H64" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="I64" s="7" t="s">
+      <c r="L72" s="26"/>
+      <c r="M72" s="27"/>
+      <c r="N72" s="27"/>
+    </row>
+    <row r="73" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="H73" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="I73" s="7" t="s">
         <v>146</v>
       </c>
-      <c r="J64" t="s">
+      <c r="J73" t="s">
         <v>150</v>
       </c>
-      <c r="L64" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="M64" s="13" t="s">
-        <v>154</v>
-      </c>
-      <c r="N64" s="15" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="65" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H65" s="5" t="s">
+      <c r="L73" s="26"/>
+      <c r="M73" s="27"/>
+      <c r="N73" s="27"/>
+    </row>
+    <row r="74" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="H74" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I65" s="7">
+      <c r="I74" s="7">
         <v>400</v>
       </c>
-      <c r="J65">
+      <c r="J74">
         <v>400</v>
       </c>
-      <c r="L65" s="10" t="s">
-        <v>54</v>
-      </c>
-      <c r="M65" s="14" t="s">
+      <c r="L74" s="26"/>
+      <c r="M74" s="27"/>
+      <c r="N74" s="27"/>
+    </row>
+    <row r="75" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="H75" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I75" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="N65" s="15" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="66" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H66" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I66" s="13" t="s">
+      <c r="J75" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="J66" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="L66" s="10" t="s">
-        <v>55</v>
-      </c>
-      <c r="M66" s="13" t="s">
-        <v>155</v>
-      </c>
-      <c r="N66" s="15" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="67" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H67" s="5" t="s">
+      <c r="L75" s="26"/>
+      <c r="M75" s="27"/>
+      <c r="N75" s="27"/>
+    </row>
+    <row r="76" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="H76" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I67" s="13" t="s">
+      <c r="I76" s="13" t="s">
         <v>152</v>
       </c>
-      <c r="J67" s="13" t="s">
+      <c r="J76" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="L67" s="10" t="s">
-        <v>56</v>
-      </c>
-      <c r="M67" s="7"/>
-      <c r="N67" s="16"/>
-    </row>
-    <row r="68" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="H68" s="5" t="s">
+      <c r="L76" s="26"/>
+      <c r="M76" s="28"/>
+      <c r="N76" s="25"/>
+    </row>
+    <row r="77" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="H77" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="I68" s="13" t="s">
+      <c r="I77" s="23" t="s">
         <v>161</v>
       </c>
-      <c r="L68" s="10" t="s">
-        <v>57</v>
-      </c>
-      <c r="M68" s="7"/>
-      <c r="N68" s="16"/>
-    </row>
-    <row r="70" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="N70" s="16" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="72" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="L72" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="M72" s="8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="73" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="L73" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="M73" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="74" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="L74" s="6" t="s">
+      <c r="L77" s="26"/>
+      <c r="M77" s="28"/>
+      <c r="N77" s="25"/>
+    </row>
+    <row r="80" spans="7:14" x14ac:dyDescent="0.25">
+      <c r="H80" s="15" t="s">
+        <v>14</v>
+      </c>
+      <c r="I80" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H81" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="I81" s="35" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="82" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H82" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="I82" s="8" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="83" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H83" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="I83" s="8" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="84" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H84" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="I84" s="9"/>
+    </row>
+    <row r="85" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H85" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="I85" s="8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="86" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H86" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="M74" s="8" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="75" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="L75" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="M75" s="8" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="76" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="L76" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="M76" s="10" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="77" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="L77" s="6" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="78" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="L78" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="79" spans="8:14" x14ac:dyDescent="0.25">
-      <c r="L79" s="6" t="s">
+      <c r="I86" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="87" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H87" s="15" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="82" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L82" s="17" t="s">
-        <v>14</v>
-      </c>
-      <c r="M82" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="83" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L83" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="M83" s="8" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="84" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L84" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="M84" s="8" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="85" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L85" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="M85" s="8" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="86" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L86" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="M86" s="9"/>
-    </row>
-    <row r="87" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L87" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="M87" s="8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="88" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L88" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="M88" s="8" t="s">
+      <c r="I87" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="88" spans="8:9" x14ac:dyDescent="0.25">
+      <c r="H88" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="I88" s="8" t="s">
         <v>170</v>
-      </c>
-    </row>
-    <row r="89" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L89" s="17" t="s">
-        <v>19</v>
-      </c>
-      <c r="M89" s="8" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="90" spans="12:13" x14ac:dyDescent="0.25">
-      <c r="L90" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="M90" s="8" t="s">
-        <v>171</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>